<commit_message>
input TUP 1 SEMUA
</commit_message>
<xml_diff>
--- a/TUP/TUP 1/Usulan TUP 1.xlsx
+++ b/TUP/TUP 1/Usulan TUP 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2023\github\TA.2023\TUP\TUP 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{381BF6E9-D985-4584-9091-BE1E8C54B3CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF66D0C-9DF0-4C91-AC4A-9E6F4323ECAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{E899FA34-6DE3-4640-B916-AC504F664995}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{E899FA34-6DE3-4640-B916-AC504F664995}"/>
   </bookViews>
   <sheets>
     <sheet name="Rekap TUP 1 Per Akun" sheetId="3" r:id="rId1"/>
@@ -3145,10 +3145,6 @@
 s.d 10 Jan 2023</t>
   </si>
   <si>
-    <t>Sisa Dana 
-s.d 10 Jan 2023</t>
-  </si>
-  <si>
     <t>Rekapitulasi Usulan TUP 1</t>
   </si>
   <si>
@@ -3194,6 +3190,10 @@
   </si>
   <si>
     <t>Ditandatangani Secara</t>
+  </si>
+  <si>
+    <t>Sisa Dana 
+s.d 16 Jan 2023</t>
   </si>
 </sst>
 </file>
@@ -4744,26 +4744,6 @@
     <xf numFmtId="0" fontId="9" fillId="40" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="41" fontId="12" fillId="10" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="12" fillId="10" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="12" fillId="10" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -4771,6 +4751,8 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4787,9 +4769,11 @@
     <xf numFmtId="0" fontId="12" fillId="10" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4816,6 +4800,22 @@
     <xf numFmtId="0" fontId="15" fillId="9" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="41" fontId="12" fillId="10" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="12" fillId="10" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="12" fillId="10" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
@@ -5739,7 +5739,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="'[5]Usulan TUP 4'!$O$534:$R$537" spid="_x0000_s3320"/>
+                  <a14:cameraTool cellRange="'[5]Usulan TUP 4'!$O$534:$R$537" spid="_x0000_s3332"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -5804,7 +5804,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$H$42:$H$43" spid="_x0000_s3321"/>
+                  <a14:cameraTool cellRange="$H$42:$H$43" spid="_x0000_s3333"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -5859,7 +5859,7 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>337970</xdr:colOff>
           <xdr:row>573</xdr:row>
-          <xdr:rowOff>4483</xdr:rowOff>
+          <xdr:rowOff>4484</xdr:rowOff>
         </xdr:to>
         <xdr:pic>
           <xdr:nvPicPr>
@@ -5874,7 +5874,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="'[5]Usulan TUP 4'!$O$534:$R$537" spid="_x0000_s5221"/>
+                  <a14:cameraTool cellRange="'[5]Usulan TUP 4'!$O$534:$R$537" spid="_x0000_s5227"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -5944,7 +5944,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="'[5]Usulan TUP 4'!$O$534:$R$537" spid="_x0000_s2181"/>
+                  <a14:cameraTool cellRange="'[5]Usulan TUP 4'!$O$534:$R$537" spid="_x0000_s2187"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -9954,8 +9954,8 @@
   </sheetPr>
   <dimension ref="A2:N45"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -10010,7 +10010,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="236" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="B9" s="236"/>
       <c r="C9" s="236"/>
@@ -10044,7 +10044,7 @@
         <v>544</v>
       </c>
       <c r="K11" s="3" t="str" cm="1">
-        <f t="array" ref="K11:L19">_xlfn.UNIQUE(MID(_xlfn._xlws.FILTER('Usulan TUP 1'!$A$15:$B$564,(LEN('Usulan TUP 1'!$B$15:$B$564)=6)*('Usulan TUP 1'!$K$15:$K$564&gt;0),""),1,11))</f>
+        <f t="array" ref="K11:L20">_xlfn.UNIQUE(MID(_xlfn._xlws.FILTER('Usulan TUP 1'!$A$15:$B$564,(LEN('Usulan TUP 1'!$B$15:$B$564)=6)*('Usulan TUP 1'!$K$15:$K$564&gt;0),""),1,11))</f>
         <v>DL.2376.AFA</v>
       </c>
       <c r="L11" s="3" t="str">
@@ -10108,7 +10108,7 @@
       </c>
       <c r="M13" s="36">
         <f>SUMIFS('Usulan TUP 1'!$K$15:$K$564,'Usulan TUP 1'!$A$15:$A$564,K13&amp;"*",'Usulan TUP 1'!$B$15:$B$564,L13)</f>
-        <v>100142000</v>
+        <v>100140000</v>
       </c>
       <c r="N13" s="15">
         <f>SUMIFS('Usulan TUP 1'!$L$15:$L$564,'Usulan TUP 1'!$A$15:$A$564,K13&amp;"*",'Usulan TUP 1'!$B$15:$B$564,L13)</f>
@@ -10200,10 +10200,10 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="227" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="B17" s="229" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="C17" s="80">
         <v>0</v>
@@ -10229,7 +10229,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="230" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="B18" s="231"/>
       <c r="C18" s="80">
@@ -10247,7 +10247,7 @@
       </c>
       <c r="M18" s="36">
         <f>SUMIFS('Usulan TUP 1'!$K$15:$K$564,'Usulan TUP 1'!$A$15:$A$564,K18&amp;"*",'Usulan TUP 1'!$B$15:$B$564,L18)</f>
-        <v>41320000</v>
+        <v>44120000</v>
       </c>
       <c r="N18" s="15">
         <f>SUMIFS('Usulan TUP 1'!$L$15:$L$564,'Usulan TUP 1'!$A$15:$A$564,K18&amp;"*",'Usulan TUP 1'!$B$15:$B$564,L18)</f>
@@ -10270,11 +10270,11 @@
         <v>WA.2378.EBD</v>
       </c>
       <c r="L19" s="3" t="str">
-        <v>524111</v>
+        <v>521219</v>
       </c>
       <c r="M19" s="36">
         <f>SUMIFS('Usulan TUP 1'!$K$15:$K$564,'Usulan TUP 1'!$A$15:$A$564,K19&amp;"*",'Usulan TUP 1'!$B$15:$B$564,L19)</f>
-        <v>26800000</v>
+        <v>250000</v>
       </c>
       <c r="N19" s="15">
         <f>SUMIFS('Usulan TUP 1'!$L$15:$L$564,'Usulan TUP 1'!$A$15:$A$564,K19&amp;"*",'Usulan TUP 1'!$B$15:$B$564,L19)</f>
@@ -10287,9 +10287,15 @@
       <c r="C20"/>
       <c r="D20"/>
       <c r="E20" s="51"/>
+      <c r="K20" s="3" t="str">
+        <v>WA.2378.EBD</v>
+      </c>
+      <c r="L20" s="3" t="str">
+        <v>524111</v>
+      </c>
       <c r="M20" s="36">
         <f>SUMIFS('Usulan TUP 1'!$K$15:$K$564,'Usulan TUP 1'!$A$15:$A$564,K20&amp;"*",'Usulan TUP 1'!$B$15:$B$564,L20)</f>
-        <v>0</v>
+        <v>31380000</v>
       </c>
       <c r="N20" s="15">
         <f>SUMIFS('Usulan TUP 1'!$L$15:$L$564,'Usulan TUP 1'!$A$15:$A$564,K20&amp;"*",'Usulan TUP 1'!$B$15:$B$564,L20)</f>
@@ -10519,17 +10525,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A6C5435-28AC-48AD-A4AE-D532A2415063}">
-  <sheetPr codeName="Sheet1">
+  <sheetPr codeName="Sheet1" filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:P965"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="B1" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="14" topLeftCell="G381" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="B1" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="14" topLeftCell="D173" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
-      <selection pane="bottomRight" activeCell="K388" sqref="K388"/>
+      <selection pane="bottomRight" activeCell="K60" sqref="K60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -10570,7 +10576,7 @@
         <v>513</v>
       </c>
       <c r="G2" s="39" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="I2" s="16"/>
       <c r="J2" s="16"/>
@@ -10587,7 +10593,7 @@
         <v>514</v>
       </c>
       <c r="G3" s="39" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="I3" s="16"/>
       <c r="J3" s="16"/>
@@ -10734,11 +10740,11 @@
     <row r="11" spans="1:16" s="39" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="40" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="C11" s="45" t="str">
         <f>": Rp. "&amp;TEXT(K15,"#.##")</f>
-        <v>: Rp. 325.602.000</v>
+        <v>: Rp. 333.230.000</v>
       </c>
       <c r="D11" s="46"/>
       <c r="E11" s="46"/>
@@ -10799,7 +10805,7 @@
         <v>971</v>
       </c>
       <c r="J13" s="218" t="s">
-        <v>972</v>
+        <v>987</v>
       </c>
       <c r="K13" s="218" t="s">
         <v>970</v>
@@ -10878,7 +10884,7 @@
       </c>
       <c r="K15" s="121">
         <f t="shared" ref="K15:L15" si="0">SUM(K16,K104)</f>
-        <v>325602000</v>
+        <v>333230000</v>
       </c>
       <c r="L15" s="121">
         <f t="shared" si="0"/>
@@ -10916,7 +10922,7 @@
       </c>
       <c r="K16" s="124">
         <f t="shared" ref="K16:L18" si="2">K17</f>
-        <v>143892000</v>
+        <v>143890000</v>
       </c>
       <c r="L16" s="124">
         <f t="shared" si="2"/>
@@ -10954,7 +10960,7 @@
       </c>
       <c r="K17" s="127">
         <f t="shared" si="2"/>
-        <v>143892000</v>
+        <v>143890000</v>
       </c>
       <c r="L17" s="127">
         <f t="shared" si="2"/>
@@ -10996,7 +11002,7 @@
       </c>
       <c r="K18" s="130">
         <f t="shared" si="2"/>
-        <v>143892000</v>
+        <v>143890000</v>
       </c>
       <c r="L18" s="130">
         <f t="shared" si="2"/>
@@ -11038,7 +11044,7 @@
       </c>
       <c r="K19" s="133">
         <f t="shared" ref="K19:L19" si="3">SUM(K20,K41,K60,K84)</f>
-        <v>143892000</v>
+        <v>143890000</v>
       </c>
       <c r="L19" s="133">
         <f t="shared" si="3"/>
@@ -11203,7 +11209,7 @@
       <c r="L23" s="145"/>
       <c r="O23" s="52"/>
     </row>
-    <row r="24" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>28</v>
       </c>
@@ -11569,7 +11575,7 @@
       <c r="L33" s="145"/>
       <c r="O33" s="52"/>
     </row>
-    <row r="34" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>43</v>
       </c>
@@ -11850,7 +11856,7 @@
       </c>
       <c r="K41" s="136">
         <f t="shared" ref="K41:L41" si="17">SUM(K42,K50)</f>
-        <v>30292000</v>
+        <v>30290000</v>
       </c>
       <c r="L41" s="136">
         <f t="shared" si="17"/>
@@ -12045,7 +12051,7 @@
       <c r="L46" s="145"/>
       <c r="O46" s="52"/>
     </row>
-    <row r="47" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>59</v>
       </c>
@@ -12182,7 +12188,7 @@
       </c>
       <c r="K50" s="151">
         <f t="shared" ref="K50:L50" si="23">SUM(K51,K56,K58)</f>
-        <v>14292000</v>
+        <v>14290000</v>
       </c>
       <c r="L50" s="151">
         <f t="shared" si="23"/>
@@ -12339,7 +12345,7 @@
       <c r="L54" s="145"/>
       <c r="O54" s="52"/>
     </row>
-    <row r="55" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="94" t="s">
         <v>595</v>
       </c>
@@ -12372,7 +12378,7 @@
       <c r="L55" s="145"/>
       <c r="O55" s="52"/>
     </row>
-    <row r="56" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>597</v>
       </c>
@@ -12410,7 +12416,7 @@
       </c>
       <c r="O56" s="52"/>
     </row>
-    <row r="57" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>598</v>
       </c>
@@ -12473,7 +12479,7 @@
       </c>
       <c r="K58" s="148">
         <f t="shared" ref="K58:L58" si="28">K59</f>
-        <v>11042000</v>
+        <v>11040000</v>
       </c>
       <c r="L58" s="148">
         <f t="shared" si="28"/>
@@ -12511,7 +12517,7 @@
         <v>66252000</v>
       </c>
       <c r="K59" s="145">
-        <v>11042000</v>
+        <v>11040000</v>
       </c>
       <c r="L59" s="145"/>
       <c r="O59" s="52"/>
@@ -12778,7 +12784,7 @@
       <c r="L66" s="145"/>
       <c r="O66" s="52"/>
     </row>
-    <row r="67" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>602</v>
       </c>
@@ -12811,7 +12817,7 @@
       <c r="L67" s="145"/>
       <c r="O67" s="52"/>
     </row>
-    <row r="68" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>76</v>
       </c>
@@ -12849,7 +12855,7 @@
       </c>
       <c r="O68" s="52"/>
     </row>
-    <row r="69" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>77</v>
       </c>
@@ -12955,7 +12961,7 @@
       <c r="L71" s="145"/>
       <c r="O71" s="52"/>
     </row>
-    <row r="72" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>80</v>
       </c>
@@ -12993,7 +12999,7 @@
       </c>
       <c r="O72" s="52"/>
     </row>
-    <row r="73" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>82</v>
       </c>
@@ -13026,7 +13032,7 @@
       <c r="L73" s="145"/>
       <c r="O73" s="52"/>
     </row>
-    <row r="74" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>83</v>
       </c>
@@ -13070,7 +13076,7 @@
       </c>
       <c r="O74" s="52"/>
     </row>
-    <row r="75" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>84</v>
       </c>
@@ -13108,7 +13114,7 @@
       </c>
       <c r="O75" s="52"/>
     </row>
-    <row r="76" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>85</v>
       </c>
@@ -13141,7 +13147,7 @@
       <c r="L76" s="145"/>
       <c r="O76" s="52"/>
     </row>
-    <row r="77" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>86</v>
       </c>
@@ -13174,7 +13180,7 @@
       <c r="L77" s="145"/>
       <c r="O77" s="52"/>
     </row>
-    <row r="78" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>608</v>
       </c>
@@ -13207,7 +13213,7 @@
       <c r="L78" s="145"/>
       <c r="O78" s="52"/>
     </row>
-    <row r="79" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>609</v>
       </c>
@@ -13240,7 +13246,7 @@
       <c r="L79" s="145"/>
       <c r="O79" s="52"/>
     </row>
-    <row r="80" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>87</v>
       </c>
@@ -13278,7 +13284,7 @@
       </c>
       <c r="O80" s="52"/>
     </row>
-    <row r="81" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>88</v>
       </c>
@@ -13311,7 +13317,7 @@
       <c r="L81" s="145"/>
       <c r="O81" s="52"/>
     </row>
-    <row r="82" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>90</v>
       </c>
@@ -13349,7 +13355,7 @@
       </c>
       <c r="O82" s="52"/>
     </row>
-    <row r="83" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>91</v>
       </c>
@@ -13422,7 +13428,7 @@
       </c>
       <c r="O84" s="52"/>
     </row>
-    <row r="85" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>97</v>
       </c>
@@ -13466,7 +13472,7 @@
       </c>
       <c r="O85" s="52"/>
     </row>
-    <row r="86" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>99</v>
       </c>
@@ -13504,7 +13510,7 @@
       </c>
       <c r="O86" s="52"/>
     </row>
-    <row r="87" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>100</v>
       </c>
@@ -13537,7 +13543,7 @@
       <c r="L87" s="145"/>
       <c r="O87" s="52"/>
     </row>
-    <row r="88" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>101</v>
       </c>
@@ -13570,7 +13576,7 @@
       <c r="L88" s="145"/>
       <c r="O88" s="52"/>
     </row>
-    <row r="89" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>102</v>
       </c>
@@ -13603,7 +13609,7 @@
       <c r="L89" s="145"/>
       <c r="O89" s="52"/>
     </row>
-    <row r="90" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>103</v>
       </c>
@@ -13636,7 +13642,7 @@
       <c r="L90" s="145"/>
       <c r="O90" s="52"/>
     </row>
-    <row r="91" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>104</v>
       </c>
@@ -13674,7 +13680,7 @@
       </c>
       <c r="O91" s="52"/>
     </row>
-    <row r="92" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>105</v>
       </c>
@@ -13789,7 +13795,7 @@
       </c>
       <c r="O94" s="52"/>
     </row>
-    <row r="95" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>615</v>
       </c>
@@ -13927,7 +13933,7 @@
       <c r="L98" s="145"/>
       <c r="O98" s="52"/>
     </row>
-    <row r="99" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="94" t="s">
         <v>619</v>
       </c>
@@ -13960,7 +13966,7 @@
       <c r="L99" s="145"/>
       <c r="O99" s="52"/>
     </row>
-    <row r="100" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>621</v>
       </c>
@@ -13998,7 +14004,7 @@
       </c>
       <c r="O100" s="52"/>
     </row>
-    <row r="101" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>622</v>
       </c>
@@ -14134,7 +14140,7 @@
       </c>
       <c r="K104" s="163">
         <f t="shared" ref="K104:L104" si="55">SUM(K105,K505)</f>
-        <v>181710000</v>
+        <v>189340000</v>
       </c>
       <c r="L104" s="163">
         <f t="shared" si="55"/>
@@ -14172,7 +14178,7 @@
       </c>
       <c r="K105" s="166">
         <f t="shared" ref="K105:L105" si="56">SUM(K106,K112,K306,K312)</f>
-        <v>181710000</v>
+        <v>189340000</v>
       </c>
       <c r="L105" s="166">
         <f t="shared" si="56"/>
@@ -14180,7 +14186,7 @@
       </c>
       <c r="O105" s="52"/>
     </row>
-    <row r="106" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>110</v>
       </c>
@@ -14222,7 +14228,7 @@
       </c>
       <c r="O106" s="52"/>
     </row>
-    <row r="107" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>113</v>
       </c>
@@ -14264,7 +14270,7 @@
       </c>
       <c r="O107" s="52"/>
     </row>
-    <row r="108" spans="1:15" ht="26" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15" ht="26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>115</v>
       </c>
@@ -14304,7 +14310,7 @@
       </c>
       <c r="O108" s="52"/>
     </row>
-    <row r="109" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>117</v>
       </c>
@@ -14348,7 +14354,7 @@
       </c>
       <c r="O109" s="52"/>
     </row>
-    <row r="110" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>118</v>
       </c>
@@ -14386,7 +14392,7 @@
       </c>
       <c r="O110" s="52"/>
     </row>
-    <row r="111" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>120</v>
       </c>
@@ -14625,7 +14631,7 @@
       </c>
       <c r="O116" s="52"/>
     </row>
-    <row r="117" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>639</v>
       </c>
@@ -14763,7 +14769,7 @@
       <c r="L120" s="145"/>
       <c r="O120" s="52"/>
     </row>
-    <row r="121" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>643</v>
       </c>
@@ -14801,7 +14807,7 @@
       </c>
       <c r="O121" s="52"/>
     </row>
-    <row r="122" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>644</v>
       </c>
@@ -14834,7 +14840,7 @@
       <c r="L122" s="145"/>
       <c r="O122" s="52"/>
     </row>
-    <row r="123" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="94" t="s">
         <v>646</v>
       </c>
@@ -14867,7 +14873,7 @@
       <c r="L123" s="145"/>
       <c r="O123" s="52"/>
     </row>
-    <row r="124" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>648</v>
       </c>
@@ -14905,7 +14911,7 @@
       </c>
       <c r="O124" s="52"/>
     </row>
-    <row r="125" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>649</v>
       </c>
@@ -14938,7 +14944,7 @@
       <c r="L125" s="145"/>
       <c r="O125" s="52"/>
     </row>
-    <row r="126" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>650</v>
       </c>
@@ -14976,7 +14982,7 @@
       </c>
       <c r="O126" s="52"/>
     </row>
-    <row r="127" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>651</v>
       </c>
@@ -15611,7 +15617,7 @@
       <c r="L143" s="145"/>
       <c r="O143" s="52"/>
     </row>
-    <row r="144" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>663</v>
       </c>
@@ -15649,7 +15655,7 @@
       </c>
       <c r="O144" s="52"/>
     </row>
-    <row r="145" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>664</v>
       </c>
@@ -16012,7 +16018,7 @@
       <c r="L154" s="145"/>
       <c r="O154" s="52"/>
     </row>
-    <row r="155" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>159</v>
       </c>
@@ -16050,7 +16056,7 @@
       </c>
       <c r="O155" s="52"/>
     </row>
-    <row r="156" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>161</v>
       </c>
@@ -17038,7 +17044,7 @@
       <c r="L182" s="145"/>
       <c r="O182" s="52"/>
     </row>
-    <row r="183" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>191</v>
       </c>
@@ -17082,7 +17088,7 @@
       </c>
       <c r="O183" s="52"/>
     </row>
-    <row r="184" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>193</v>
       </c>
@@ -17120,7 +17126,7 @@
       </c>
       <c r="O184" s="52"/>
     </row>
-    <row r="185" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>194</v>
       </c>
@@ -17153,7 +17159,7 @@
       <c r="L185" s="145"/>
       <c r="O185" s="52"/>
     </row>
-    <row r="186" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>195</v>
       </c>
@@ -17186,7 +17192,7 @@
       <c r="L186" s="145"/>
       <c r="O186" s="52"/>
     </row>
-    <row r="187" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>196</v>
       </c>
@@ -17219,7 +17225,7 @@
       <c r="L187" s="145"/>
       <c r="O187" s="52"/>
     </row>
-    <row r="188" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>679</v>
       </c>
@@ -17252,7 +17258,7 @@
       <c r="L188" s="145"/>
       <c r="O188" s="52"/>
     </row>
-    <row r="189" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>197</v>
       </c>
@@ -17290,7 +17296,7 @@
       </c>
       <c r="O189" s="52"/>
     </row>
-    <row r="190" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>198</v>
       </c>
@@ -17323,7 +17329,7 @@
       <c r="L190" s="145"/>
       <c r="O190" s="52"/>
     </row>
-    <row r="191" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>199</v>
       </c>
@@ -17361,7 +17367,7 @@
       </c>
       <c r="O191" s="52"/>
     </row>
-    <row r="192" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>200</v>
       </c>
@@ -17394,7 +17400,7 @@
       <c r="L192" s="145"/>
       <c r="O192" s="52"/>
     </row>
-    <row r="193" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>201</v>
       </c>
@@ -17432,7 +17438,7 @@
       </c>
       <c r="O193" s="52"/>
     </row>
-    <row r="194" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>202</v>
       </c>
@@ -17582,7 +17588,7 @@
       <c r="L197" s="145"/>
       <c r="O197" s="52"/>
     </row>
-    <row r="198" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>208</v>
       </c>
@@ -17983,7 +17989,7 @@
       <c r="L208" s="145"/>
       <c r="O208" s="52"/>
     </row>
-    <row r="209" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
         <v>219</v>
       </c>
@@ -18016,7 +18022,7 @@
       <c r="L209" s="145"/>
       <c r="O209" s="52"/>
     </row>
-    <row r="210" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>220</v>
       </c>
@@ -18049,7 +18055,7 @@
       <c r="L210" s="145"/>
       <c r="O210" s="52"/>
     </row>
-    <row r="211" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
         <v>221</v>
       </c>
@@ -18087,7 +18093,7 @@
       </c>
       <c r="O211" s="52"/>
     </row>
-    <row r="212" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>222</v>
       </c>
@@ -18120,7 +18126,7 @@
       <c r="L212" s="145"/>
       <c r="O212" s="52"/>
     </row>
-    <row r="213" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>223</v>
       </c>
@@ -18164,7 +18170,7 @@
       </c>
       <c r="O213" s="52"/>
     </row>
-    <row r="214" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
         <v>225</v>
       </c>
@@ -18202,7 +18208,7 @@
       </c>
       <c r="O214" s="52"/>
     </row>
-    <row r="215" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
         <v>226</v>
       </c>
@@ -18235,7 +18241,7 @@
       <c r="L215" s="145"/>
       <c r="O215" s="52"/>
     </row>
-    <row r="216" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>227</v>
       </c>
@@ -18268,7 +18274,7 @@
       <c r="L216" s="145"/>
       <c r="O216" s="52"/>
     </row>
-    <row r="217" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
         <v>228</v>
       </c>
@@ -18301,7 +18307,7 @@
       <c r="L217" s="145"/>
       <c r="O217" s="52"/>
     </row>
-    <row r="218" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>229</v>
       </c>
@@ -18334,7 +18340,7 @@
       <c r="L218" s="145"/>
       <c r="O218" s="52"/>
     </row>
-    <row r="219" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
         <v>230</v>
       </c>
@@ -18372,7 +18378,7 @@
       </c>
       <c r="O219" s="52"/>
     </row>
-    <row r="220" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>231</v>
       </c>
@@ -18405,7 +18411,7 @@
       <c r="L220" s="145"/>
       <c r="O220" s="52"/>
     </row>
-    <row r="221" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>232</v>
       </c>
@@ -18447,7 +18453,7 @@
       </c>
       <c r="O221" s="52"/>
     </row>
-    <row r="222" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:15" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>557</v>
       </c>
@@ -18487,7 +18493,7 @@
       </c>
       <c r="O222" s="52"/>
     </row>
-    <row r="223" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
         <v>688</v>
       </c>
@@ -18531,7 +18537,7 @@
       </c>
       <c r="O223" s="52"/>
     </row>
-    <row r="224" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
         <v>690</v>
       </c>
@@ -18569,7 +18575,7 @@
       </c>
       <c r="O224" s="52"/>
     </row>
-    <row r="225" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>692</v>
       </c>
@@ -18604,7 +18610,7 @@
       <c r="L225" s="145"/>
       <c r="O225" s="52"/>
     </row>
-    <row r="226" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>695</v>
       </c>
@@ -18642,7 +18648,7 @@
       </c>
       <c r="O226" s="52"/>
     </row>
-    <row r="227" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>697</v>
       </c>
@@ -18677,7 +18683,7 @@
       <c r="L227" s="145"/>
       <c r="O227" s="52"/>
     </row>
-    <row r="228" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>699</v>
       </c>
@@ -18715,7 +18721,7 @@
       </c>
       <c r="O228" s="52"/>
     </row>
-    <row r="229" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
         <v>701</v>
       </c>
@@ -18750,7 +18756,7 @@
       <c r="L229" s="145"/>
       <c r="O229" s="52"/>
     </row>
-    <row r="230" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>703</v>
       </c>
@@ -18788,7 +18794,7 @@
       </c>
       <c r="O230" s="52"/>
     </row>
-    <row r="231" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
         <v>705</v>
       </c>
@@ -18823,7 +18829,7 @@
       <c r="L231" s="145"/>
       <c r="O231" s="52"/>
     </row>
-    <row r="232" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
         <v>707</v>
       </c>
@@ -18861,7 +18867,7 @@
       </c>
       <c r="O232" s="52"/>
     </row>
-    <row r="233" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
         <v>709</v>
       </c>
@@ -18896,7 +18902,7 @@
       <c r="L233" s="145"/>
       <c r="O233" s="52"/>
     </row>
-    <row r="234" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
         <v>711</v>
       </c>
@@ -18934,7 +18940,7 @@
       </c>
       <c r="O234" s="52"/>
     </row>
-    <row r="235" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
         <v>713</v>
       </c>
@@ -18969,7 +18975,7 @@
       <c r="L235" s="145"/>
       <c r="O235" s="52"/>
     </row>
-    <row r="236" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>715</v>
       </c>
@@ -19007,7 +19013,7 @@
       </c>
       <c r="O236" s="52"/>
     </row>
-    <row r="237" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
         <v>717</v>
       </c>
@@ -19042,7 +19048,7 @@
       <c r="L237" s="145"/>
       <c r="O237" s="52"/>
     </row>
-    <row r="238" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>719</v>
       </c>
@@ -19080,7 +19086,7 @@
       </c>
       <c r="O238" s="52"/>
     </row>
-    <row r="239" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
         <v>721</v>
       </c>
@@ -19115,7 +19121,7 @@
       <c r="L239" s="145"/>
       <c r="O239" s="52"/>
     </row>
-    <row r="240" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
         <v>723</v>
       </c>
@@ -19153,7 +19159,7 @@
       </c>
       <c r="O240" s="52"/>
     </row>
-    <row r="241" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
         <v>725</v>
       </c>
@@ -19186,7 +19192,7 @@
       <c r="L241" s="145"/>
       <c r="O241" s="52"/>
     </row>
-    <row r="242" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
         <v>727</v>
       </c>
@@ -19224,7 +19230,7 @@
       </c>
       <c r="O242" s="52"/>
     </row>
-    <row r="243" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
         <v>729</v>
       </c>
@@ -19259,7 +19265,7 @@
       <c r="L243" s="145"/>
       <c r="O243" s="52"/>
     </row>
-    <row r="244" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
         <v>731</v>
       </c>
@@ -19297,7 +19303,7 @@
       </c>
       <c r="O244" s="52"/>
     </row>
-    <row r="245" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
         <v>734</v>
       </c>
@@ -19330,7 +19336,7 @@
       <c r="L245" s="145"/>
       <c r="O245" s="52"/>
     </row>
-    <row r="246" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
         <v>736</v>
       </c>
@@ -19368,7 +19374,7 @@
       </c>
       <c r="O246" s="52"/>
     </row>
-    <row r="247" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
         <v>738</v>
       </c>
@@ -19401,7 +19407,7 @@
       <c r="L247" s="145"/>
       <c r="O247" s="52"/>
     </row>
-    <row r="248" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
         <v>235</v>
       </c>
@@ -19441,7 +19447,7 @@
       </c>
       <c r="O248" s="52"/>
     </row>
-    <row r="249" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
         <v>238</v>
       </c>
@@ -19485,7 +19491,7 @@
       </c>
       <c r="O249" s="52"/>
     </row>
-    <row r="250" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
         <v>241</v>
       </c>
@@ -19523,7 +19529,7 @@
       </c>
       <c r="O250" s="52"/>
     </row>
-    <row r="251" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
         <v>243</v>
       </c>
@@ -19556,7 +19562,7 @@
       <c r="L251" s="145"/>
       <c r="O251" s="52"/>
     </row>
-    <row r="252" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>244</v>
       </c>
@@ -19589,7 +19595,7 @@
       <c r="L252" s="145"/>
       <c r="O252" s="52"/>
     </row>
-    <row r="253" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
         <v>245</v>
       </c>
@@ -19622,7 +19628,7 @@
       <c r="L253" s="145"/>
       <c r="O253" s="52"/>
     </row>
-    <row r="254" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
         <v>246</v>
       </c>
@@ -19655,7 +19661,7 @@
       <c r="L254" s="145"/>
       <c r="O254" s="52"/>
     </row>
-    <row r="255" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
         <v>247</v>
       </c>
@@ -19688,7 +19694,7 @@
       <c r="L255" s="145"/>
       <c r="O255" s="52"/>
     </row>
-    <row r="256" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>249</v>
       </c>
@@ -19721,7 +19727,7 @@
       <c r="L256" s="145"/>
       <c r="O256" s="52"/>
     </row>
-    <row r="257" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
         <v>250</v>
       </c>
@@ -19754,7 +19760,7 @@
       <c r="L257" s="145"/>
       <c r="O257" s="52"/>
     </row>
-    <row r="258" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>251</v>
       </c>
@@ -19787,7 +19793,7 @@
       <c r="L258" s="145"/>
       <c r="O258" s="52"/>
     </row>
-    <row r="259" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
         <v>252</v>
       </c>
@@ -19820,7 +19826,7 @@
       <c r="L259" s="145"/>
       <c r="O259" s="52"/>
     </row>
-    <row r="260" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
         <v>751</v>
       </c>
@@ -19853,7 +19859,7 @@
       <c r="L260" s="145"/>
       <c r="O260" s="52"/>
     </row>
-    <row r="261" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
         <v>753</v>
       </c>
@@ -19891,7 +19897,7 @@
       </c>
       <c r="O261" s="52"/>
     </row>
-    <row r="262" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
         <v>756</v>
       </c>
@@ -19922,7 +19928,7 @@
       <c r="L262" s="145"/>
       <c r="O262" s="52"/>
     </row>
-    <row r="263" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
         <v>253</v>
       </c>
@@ -19958,7 +19964,7 @@
       </c>
       <c r="O263" s="52"/>
     </row>
-    <row r="264" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" s="94" t="s">
         <v>254</v>
       </c>
@@ -19989,7 +19995,7 @@
       <c r="L264" s="145"/>
       <c r="O264" s="52"/>
     </row>
-    <row r="265" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
         <v>255</v>
       </c>
@@ -20020,7 +20026,7 @@
       <c r="L265" s="145"/>
       <c r="O265" s="52"/>
     </row>
-    <row r="266" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
         <v>256</v>
       </c>
@@ -20051,7 +20057,7 @@
       <c r="L266" s="145"/>
       <c r="O266" s="52"/>
     </row>
-    <row r="267" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
         <v>257</v>
       </c>
@@ -20082,7 +20088,7 @@
       <c r="L267" s="145"/>
       <c r="O267" s="52"/>
     </row>
-    <row r="268" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
         <v>258</v>
       </c>
@@ -20113,7 +20119,7 @@
       <c r="L268" s="145"/>
       <c r="O268" s="52"/>
     </row>
-    <row r="269" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
         <v>260</v>
       </c>
@@ -20144,7 +20150,7 @@
       <c r="L269" s="145"/>
       <c r="O269" s="52"/>
     </row>
-    <row r="270" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
         <v>261</v>
       </c>
@@ -20175,7 +20181,7 @@
       <c r="L270" s="145"/>
       <c r="O270" s="52"/>
     </row>
-    <row r="271" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
         <v>263</v>
       </c>
@@ -20206,7 +20212,7 @@
       <c r="L271" s="145"/>
       <c r="O271" s="52"/>
     </row>
-    <row r="272" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
         <v>265</v>
       </c>
@@ -20237,7 +20243,7 @@
       <c r="L272" s="145"/>
       <c r="O272" s="52"/>
     </row>
-    <row r="273" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
         <v>266</v>
       </c>
@@ -20279,7 +20285,7 @@
       </c>
       <c r="O273" s="52"/>
     </row>
-    <row r="274" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
         <v>269</v>
       </c>
@@ -20315,7 +20321,7 @@
       </c>
       <c r="O274" s="52"/>
     </row>
-    <row r="275" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
         <v>271</v>
       </c>
@@ -20346,7 +20352,7 @@
       <c r="L275" s="145"/>
       <c r="O275" s="52"/>
     </row>
-    <row r="276" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
         <v>272</v>
       </c>
@@ -20382,7 +20388,7 @@
       </c>
       <c r="O276" s="52"/>
     </row>
-    <row r="277" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
         <v>273</v>
       </c>
@@ -20413,7 +20419,7 @@
       <c r="L277" s="145"/>
       <c r="O277" s="52"/>
     </row>
-    <row r="278" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
         <v>274</v>
       </c>
@@ -20444,7 +20450,7 @@
       <c r="L278" s="145"/>
       <c r="O278" s="52"/>
     </row>
-    <row r="279" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
         <v>275</v>
       </c>
@@ -20486,7 +20492,7 @@
       </c>
       <c r="O279" s="52"/>
     </row>
-    <row r="280" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
         <v>278</v>
       </c>
@@ -20522,7 +20528,7 @@
       </c>
       <c r="O280" s="52"/>
     </row>
-    <row r="281" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
         <v>280</v>
       </c>
@@ -20553,7 +20559,7 @@
       <c r="L281" s="145"/>
       <c r="O281" s="52"/>
     </row>
-    <row r="282" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
         <v>281</v>
       </c>
@@ -20584,7 +20590,7 @@
       <c r="L282" s="145"/>
       <c r="O282" s="52"/>
     </row>
-    <row r="283" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
         <v>282</v>
       </c>
@@ -20615,7 +20621,7 @@
       <c r="L283" s="145"/>
       <c r="O283" s="52"/>
     </row>
-    <row r="284" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
         <v>283</v>
       </c>
@@ -20646,7 +20652,7 @@
       <c r="L284" s="145"/>
       <c r="O284" s="52"/>
     </row>
-    <row r="285" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
         <v>284</v>
       </c>
@@ -20677,7 +20683,7 @@
       <c r="L285" s="145"/>
       <c r="O285" s="52"/>
     </row>
-    <row r="286" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
         <v>285</v>
       </c>
@@ -20708,7 +20714,7 @@
       <c r="L286" s="145"/>
       <c r="O286" s="52"/>
     </row>
-    <row r="287" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
         <v>286</v>
       </c>
@@ -20739,7 +20745,7 @@
       <c r="L287" s="145"/>
       <c r="O287" s="52"/>
     </row>
-    <row r="288" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
         <v>287</v>
       </c>
@@ -20770,7 +20776,7 @@
       <c r="L288" s="145"/>
       <c r="O288" s="52"/>
     </row>
-    <row r="289" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
         <v>288</v>
       </c>
@@ -20801,7 +20807,7 @@
       <c r="L289" s="145"/>
       <c r="O289" s="52"/>
     </row>
-    <row r="290" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
         <v>289</v>
       </c>
@@ -20837,7 +20843,7 @@
       </c>
       <c r="O290" s="52"/>
     </row>
-    <row r="291" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
         <v>291</v>
       </c>
@@ -20868,7 +20874,7 @@
       <c r="L291" s="145"/>
       <c r="O291" s="52"/>
     </row>
-    <row r="292" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
         <v>293</v>
       </c>
@@ -20910,7 +20916,7 @@
       </c>
       <c r="O292" s="52"/>
     </row>
-    <row r="293" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
         <v>296</v>
       </c>
@@ -20946,7 +20952,7 @@
       </c>
       <c r="O293" s="52"/>
     </row>
-    <row r="294" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
         <v>297</v>
       </c>
@@ -20977,7 +20983,7 @@
       <c r="L294" s="145"/>
       <c r="O294" s="52"/>
     </row>
-    <row r="295" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
         <v>299</v>
       </c>
@@ -21013,7 +21019,7 @@
       </c>
       <c r="O295" s="52"/>
     </row>
-    <row r="296" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
         <v>301</v>
       </c>
@@ -21044,7 +21050,7 @@
       <c r="L296" s="145"/>
       <c r="O296" s="52"/>
     </row>
-    <row r="297" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
         <v>302</v>
       </c>
@@ -21075,7 +21081,7 @@
       <c r="L297" s="145"/>
       <c r="O297" s="52"/>
     </row>
-    <row r="298" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
         <v>303</v>
       </c>
@@ -21106,7 +21112,7 @@
       <c r="L298" s="145"/>
       <c r="O298" s="52"/>
     </row>
-    <row r="299" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
         <v>304</v>
       </c>
@@ -21137,7 +21143,7 @@
       <c r="L299" s="145"/>
       <c r="O299" s="52"/>
     </row>
-    <row r="300" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300" s="1" t="s">
         <v>305</v>
       </c>
@@ -21168,7 +21174,7 @@
       <c r="L300" s="145"/>
       <c r="O300" s="52"/>
     </row>
-    <row r="301" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301" s="1" t="s">
         <v>306</v>
       </c>
@@ -21199,7 +21205,7 @@
       <c r="L301" s="145"/>
       <c r="O301" s="52"/>
     </row>
-    <row r="302" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302" s="1" t="s">
         <v>307</v>
       </c>
@@ -21230,7 +21236,7 @@
       <c r="L302" s="145"/>
       <c r="O302" s="52"/>
     </row>
-    <row r="303" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303" s="1" t="s">
         <v>308</v>
       </c>
@@ -21261,7 +21267,7 @@
       <c r="L303" s="145"/>
       <c r="O303" s="52"/>
     </row>
-    <row r="304" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304" s="1" t="s">
         <v>309</v>
       </c>
@@ -21292,7 +21298,7 @@
       <c r="L304" s="145"/>
       <c r="O304" s="52"/>
     </row>
-    <row r="305" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305" s="1" t="s">
         <v>310</v>
       </c>
@@ -21325,7 +21331,7 @@
       <c r="L305" s="145"/>
       <c r="O305" s="52"/>
     </row>
-    <row r="306" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306" s="1" t="s">
         <v>311</v>
       </c>
@@ -21367,7 +21373,7 @@
       </c>
       <c r="O306" s="52"/>
     </row>
-    <row r="307" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307" s="1" t="s">
         <v>313</v>
       </c>
@@ -21409,7 +21415,7 @@
       </c>
       <c r="O307" s="52"/>
     </row>
-    <row r="308" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308" s="1" t="s">
         <v>799</v>
       </c>
@@ -21449,7 +21455,7 @@
       </c>
       <c r="O308" s="52"/>
     </row>
-    <row r="309" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309" s="1" t="s">
         <v>802</v>
       </c>
@@ -21493,7 +21499,7 @@
       </c>
       <c r="O309" s="52"/>
     </row>
-    <row r="310" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310" s="1" t="s">
         <v>803</v>
       </c>
@@ -21531,7 +21537,7 @@
       </c>
       <c r="O310" s="52"/>
     </row>
-    <row r="311" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311" s="1" t="s">
         <v>804</v>
       </c>
@@ -21598,7 +21604,7 @@
       </c>
       <c r="K312" s="206">
         <f t="shared" ref="K312:L312" si="170">SUM(K313,K384,K432)</f>
-        <v>68120000</v>
+        <v>75750000</v>
       </c>
       <c r="L312" s="206">
         <f t="shared" si="170"/>
@@ -21770,7 +21776,7 @@
       </c>
       <c r="O316" s="52"/>
     </row>
-    <row r="317" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317" s="1" t="s">
         <v>326</v>
       </c>
@@ -21908,7 +21914,7 @@
       <c r="L320" s="145"/>
       <c r="O320" s="52"/>
     </row>
-    <row r="321" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321" s="1" t="s">
         <v>812</v>
       </c>
@@ -21941,7 +21947,7 @@
       <c r="L321" s="145"/>
       <c r="O321" s="52"/>
     </row>
-    <row r="322" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322" s="1" t="s">
         <v>327</v>
       </c>
@@ -21979,7 +21985,7 @@
       </c>
       <c r="O322" s="52"/>
     </row>
-    <row r="323" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A323" s="1" t="s">
         <v>328</v>
       </c>
@@ -22012,7 +22018,7 @@
       <c r="L323" s="145"/>
       <c r="O323" s="52"/>
     </row>
-    <row r="324" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324" s="1" t="s">
         <v>329</v>
       </c>
@@ -22050,7 +22056,7 @@
       </c>
       <c r="O324" s="52"/>
     </row>
-    <row r="325" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325" s="1" t="s">
         <v>330</v>
       </c>
@@ -22165,7 +22171,7 @@
       </c>
       <c r="O327" s="52"/>
     </row>
-    <row r="328" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328" s="1" t="s">
         <v>334</v>
       </c>
@@ -22303,7 +22309,7 @@
       <c r="L331" s="145"/>
       <c r="O331" s="52"/>
     </row>
-    <row r="332" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A332" s="1" t="s">
         <v>817</v>
       </c>
@@ -22336,7 +22342,7 @@
       <c r="L332" s="145"/>
       <c r="O332" s="52"/>
     </row>
-    <row r="333" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A333" s="1" t="s">
         <v>336</v>
       </c>
@@ -22374,7 +22380,7 @@
       </c>
       <c r="O333" s="52"/>
     </row>
-    <row r="334" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A334" s="1" t="s">
         <v>337</v>
       </c>
@@ -22407,7 +22413,7 @@
       <c r="L334" s="145"/>
       <c r="O334" s="52"/>
     </row>
-    <row r="335" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A335" s="1" t="s">
         <v>338</v>
       </c>
@@ -22445,7 +22451,7 @@
       </c>
       <c r="O335" s="52"/>
     </row>
-    <row r="336" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336" s="1" t="s">
         <v>339</v>
       </c>
@@ -22478,7 +22484,7 @@
       <c r="L336" s="145"/>
       <c r="O336" s="52"/>
     </row>
-    <row r="337" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337" s="1" t="s">
         <v>340</v>
       </c>
@@ -22516,7 +22522,7 @@
       </c>
       <c r="O337" s="52"/>
     </row>
-    <row r="338" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338" s="1" t="s">
         <v>341</v>
       </c>
@@ -22631,7 +22637,7 @@
       </c>
       <c r="O340" s="52"/>
     </row>
-    <row r="341" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A341" s="1" t="s">
         <v>344</v>
       </c>
@@ -22769,7 +22775,7 @@
       <c r="L344" s="145"/>
       <c r="O344" s="52"/>
     </row>
-    <row r="345" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A345" s="1" t="s">
         <v>822</v>
       </c>
@@ -22802,7 +22808,7 @@
       <c r="L345" s="145"/>
       <c r="O345" s="52"/>
     </row>
-    <row r="346" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346" s="1" t="s">
         <v>823</v>
       </c>
@@ -22840,7 +22846,7 @@
       </c>
       <c r="O346" s="52"/>
     </row>
-    <row r="347" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A347" s="1" t="s">
         <v>824</v>
       </c>
@@ -22873,7 +22879,7 @@
       <c r="L347" s="145"/>
       <c r="O347" s="52"/>
     </row>
-    <row r="348" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348" s="1" t="s">
         <v>825</v>
       </c>
@@ -22911,7 +22917,7 @@
       </c>
       <c r="O348" s="52"/>
     </row>
-    <row r="349" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A349" s="1" t="s">
         <v>826</v>
       </c>
@@ -22944,7 +22950,7 @@
       <c r="L349" s="145"/>
       <c r="O349" s="52"/>
     </row>
-    <row r="350" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A350" s="1" t="s">
         <v>346</v>
       </c>
@@ -22982,7 +22988,7 @@
       </c>
       <c r="O350" s="52"/>
     </row>
-    <row r="351" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A351" s="1" t="s">
         <v>347</v>
       </c>
@@ -23097,7 +23103,7 @@
       </c>
       <c r="O353" s="52"/>
     </row>
-    <row r="354" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A354" s="1" t="s">
         <v>830</v>
       </c>
@@ -23235,7 +23241,7 @@
       <c r="L357" s="145"/>
       <c r="O357" s="52"/>
     </row>
-    <row r="358" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A358" s="1" t="s">
         <v>349</v>
       </c>
@@ -23273,7 +23279,7 @@
       </c>
       <c r="O358" s="52"/>
     </row>
-    <row r="359" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A359" s="1" t="s">
         <v>350</v>
       </c>
@@ -23388,7 +23394,7 @@
       </c>
       <c r="O361" s="52"/>
     </row>
-    <row r="362" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A362" s="1" t="s">
         <v>838</v>
       </c>
@@ -23526,7 +23532,7 @@
       <c r="L365" s="145"/>
       <c r="O365" s="52"/>
     </row>
-    <row r="366" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A366" s="1" t="s">
         <v>842</v>
       </c>
@@ -23564,7 +23570,7 @@
       </c>
       <c r="O366" s="52"/>
     </row>
-    <row r="367" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A367" s="1" t="s">
         <v>843</v>
       </c>
@@ -23597,7 +23603,7 @@
       <c r="L367" s="145"/>
       <c r="O367" s="52"/>
     </row>
-    <row r="368" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A368" s="1" t="s">
         <v>845</v>
       </c>
@@ -23641,7 +23647,7 @@
       </c>
       <c r="O368" s="52"/>
     </row>
-    <row r="369" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A369" s="1" t="s">
         <v>847</v>
       </c>
@@ -23679,7 +23685,7 @@
       </c>
       <c r="O369" s="52"/>
     </row>
-    <row r="370" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A370" s="1" t="s">
         <v>848</v>
       </c>
@@ -23712,7 +23718,7 @@
       <c r="L370" s="145"/>
       <c r="O370" s="52"/>
     </row>
-    <row r="371" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A371" s="1" t="s">
         <v>849</v>
       </c>
@@ -23745,7 +23751,7 @@
       <c r="L371" s="145"/>
       <c r="O371" s="52"/>
     </row>
-    <row r="372" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A372" s="1" t="s">
         <v>850</v>
       </c>
@@ -23778,7 +23784,7 @@
       <c r="L372" s="145"/>
       <c r="O372" s="52"/>
     </row>
-    <row r="373" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A373" s="1" t="s">
         <v>851</v>
       </c>
@@ -23811,7 +23817,7 @@
       <c r="L373" s="145"/>
       <c r="O373" s="52"/>
     </row>
-    <row r="374" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A374" s="1" t="s">
         <v>852</v>
       </c>
@@ -23844,7 +23850,7 @@
       <c r="L374" s="145"/>
       <c r="O374" s="52"/>
     </row>
-    <row r="375" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A375" s="1" t="s">
         <v>854</v>
       </c>
@@ -23877,7 +23883,7 @@
       <c r="L375" s="145"/>
       <c r="O375" s="52"/>
     </row>
-    <row r="376" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A376" s="1" t="s">
         <v>856</v>
       </c>
@@ -23915,7 +23921,7 @@
       </c>
       <c r="O376" s="52"/>
     </row>
-    <row r="377" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A377" s="1" t="s">
         <v>857</v>
       </c>
@@ -23948,7 +23954,7 @@
       <c r="L377" s="145"/>
       <c r="O377" s="52"/>
     </row>
-    <row r="378" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A378" s="1" t="s">
         <v>858</v>
       </c>
@@ -23986,7 +23992,7 @@
       </c>
       <c r="O378" s="52"/>
     </row>
-    <row r="379" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A379" s="1" t="s">
         <v>859</v>
       </c>
@@ -24019,7 +24025,7 @@
       <c r="L379" s="145"/>
       <c r="O379" s="52"/>
     </row>
-    <row r="380" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A380" s="1" t="s">
         <v>861</v>
       </c>
@@ -24057,7 +24063,7 @@
       </c>
       <c r="O380" s="52"/>
     </row>
-    <row r="381" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A381" s="1" t="s">
         <v>862</v>
       </c>
@@ -24090,7 +24096,7 @@
       <c r="L381" s="145"/>
       <c r="O381" s="52"/>
     </row>
-    <row r="382" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A382" s="1" t="s">
         <v>864</v>
       </c>
@@ -24123,7 +24129,7 @@
       <c r="L382" s="145"/>
       <c r="O382" s="52"/>
     </row>
-    <row r="383" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A383" s="1" t="s">
         <v>866</v>
       </c>
@@ -24190,7 +24196,7 @@
       </c>
       <c r="K384" s="133">
         <f t="shared" ref="K384:L384" si="212">SUM(K385,K422)</f>
-        <v>0</v>
+        <v>18130000</v>
       </c>
       <c r="L384" s="133">
         <f t="shared" si="212"/>
@@ -24230,7 +24236,7 @@
       </c>
       <c r="K385" s="136">
         <f t="shared" ref="K385:L385" si="213">SUM(K386,K397,K411)</f>
-        <v>0</v>
+        <v>6450000</v>
       </c>
       <c r="L385" s="136">
         <f t="shared" si="213"/>
@@ -24268,7 +24274,7 @@
       </c>
       <c r="K386" s="139">
         <f t="shared" ref="K386:L386" si="214">SUM(K387,K393,K395)</f>
-        <v>0</v>
+        <v>5250000</v>
       </c>
       <c r="L386" s="139">
         <f t="shared" si="214"/>
@@ -24312,7 +24318,7 @@
       </c>
       <c r="K387" s="142">
         <f t="shared" ref="K387:L387" si="215">SUM(K388:K392)</f>
-        <v>0</v>
+        <v>5000000</v>
       </c>
       <c r="L387" s="142">
         <f t="shared" si="215"/>
@@ -24349,7 +24355,9 @@
         <f t="shared" ref="J388:J392" si="217">G388-I388</f>
         <v>21000000</v>
       </c>
-      <c r="K388" s="145"/>
+      <c r="K388" s="145">
+        <v>750000</v>
+      </c>
       <c r="L388" s="145"/>
       <c r="O388" s="52"/>
     </row>
@@ -24382,7 +24390,9 @@
         <f t="shared" si="217"/>
         <v>6000000</v>
       </c>
-      <c r="K389" s="145"/>
+      <c r="K389" s="145">
+        <v>1500000</v>
+      </c>
       <c r="L389" s="145"/>
       <c r="O389" s="52"/>
     </row>
@@ -24415,7 +24425,9 @@
         <f t="shared" si="217"/>
         <v>6000000</v>
       </c>
-      <c r="K390" s="145"/>
+      <c r="K390" s="145">
+        <v>1500000</v>
+      </c>
       <c r="L390" s="145"/>
       <c r="O390" s="52"/>
     </row>
@@ -24448,7 +24460,9 @@
         <f t="shared" si="217"/>
         <v>4000000</v>
       </c>
-      <c r="K391" s="145"/>
+      <c r="K391" s="145">
+        <v>1000000</v>
+      </c>
       <c r="L391" s="145"/>
       <c r="O391" s="52"/>
     </row>
@@ -24481,7 +24495,9 @@
         <f t="shared" si="217"/>
         <v>3000000</v>
       </c>
-      <c r="K392" s="145"/>
+      <c r="K392" s="145">
+        <v>250000</v>
+      </c>
       <c r="L392" s="145"/>
       <c r="O392" s="52"/>
     </row>
@@ -24515,7 +24531,7 @@
       </c>
       <c r="K393" s="148">
         <f t="shared" ref="K393:L393" si="218">K394</f>
-        <v>0</v>
+        <v>250000</v>
       </c>
       <c r="L393" s="148">
         <f t="shared" si="218"/>
@@ -24552,11 +24568,13 @@
         <f>G394-I394</f>
         <v>1000000</v>
       </c>
-      <c r="K394" s="145"/>
+      <c r="K394" s="145">
+        <v>250000</v>
+      </c>
       <c r="L394" s="145"/>
       <c r="O394" s="52"/>
     </row>
-    <row r="395" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A395" s="1" t="s">
         <v>364</v>
       </c>
@@ -24594,7 +24612,7 @@
       </c>
       <c r="O395" s="52"/>
     </row>
-    <row r="396" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A396" s="1" t="s">
         <v>365</v>
       </c>
@@ -24657,7 +24675,7 @@
       </c>
       <c r="K397" s="151">
         <f t="shared" ref="K397:L397" si="220">SUM(K398,K404,K407,K409)</f>
-        <v>0</v>
+        <v>1200000</v>
       </c>
       <c r="L397" s="151">
         <f t="shared" si="220"/>
@@ -24701,7 +24719,7 @@
       </c>
       <c r="K398" s="148">
         <f t="shared" ref="K398:L398" si="221">SUM(K399:K403)</f>
-        <v>0</v>
+        <v>1200000</v>
       </c>
       <c r="L398" s="148">
         <f t="shared" si="221"/>
@@ -24738,11 +24756,13 @@
         <f t="shared" ref="J399:J403" si="223">G399-I399</f>
         <v>13500000</v>
       </c>
-      <c r="K399" s="145"/>
+      <c r="K399" s="145">
+        <v>1200000</v>
+      </c>
       <c r="L399" s="145"/>
       <c r="O399" s="52"/>
     </row>
-    <row r="400" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A400" s="1" t="s">
         <v>369</v>
       </c>
@@ -24775,7 +24795,7 @@
       <c r="L400" s="145"/>
       <c r="O400" s="52"/>
     </row>
-    <row r="401" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A401" s="1" t="s">
         <v>370</v>
       </c>
@@ -24808,7 +24828,7 @@
       <c r="L401" s="145"/>
       <c r="O401" s="52"/>
     </row>
-    <row r="402" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A402" s="1" t="s">
         <v>371</v>
       </c>
@@ -24841,7 +24861,7 @@
       <c r="L402" s="145"/>
       <c r="O402" s="52"/>
     </row>
-    <row r="403" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A403" s="1" t="s">
         <v>372</v>
       </c>
@@ -24874,7 +24894,7 @@
       <c r="L403" s="145"/>
       <c r="O403" s="52"/>
     </row>
-    <row r="404" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A404" s="1" t="s">
         <v>373</v>
       </c>
@@ -24912,7 +24932,7 @@
       </c>
       <c r="O404" s="52"/>
     </row>
-    <row r="405" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A405" s="1" t="s">
         <v>374</v>
       </c>
@@ -24945,7 +24965,7 @@
       <c r="L405" s="145"/>
       <c r="O405" s="52"/>
     </row>
-    <row r="406" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A406" s="1" t="s">
         <v>874</v>
       </c>
@@ -24978,7 +24998,7 @@
       <c r="L406" s="145"/>
       <c r="O406" s="52"/>
     </row>
-    <row r="407" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A407" s="1" t="s">
         <v>876</v>
       </c>
@@ -25016,7 +25036,7 @@
       </c>
       <c r="O407" s="52"/>
     </row>
-    <row r="408" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A408" s="1" t="s">
         <v>877</v>
       </c>
@@ -25049,7 +25069,7 @@
       <c r="L408" s="145"/>
       <c r="O408" s="52"/>
     </row>
-    <row r="409" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A409" s="1" t="s">
         <v>375</v>
       </c>
@@ -25087,7 +25107,7 @@
       </c>
       <c r="O409" s="52"/>
     </row>
-    <row r="410" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A410" s="1" t="s">
         <v>376</v>
       </c>
@@ -25120,7 +25140,7 @@
       <c r="L410" s="145"/>
       <c r="O410" s="52"/>
     </row>
-    <row r="411" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A411" s="1" t="s">
         <v>377</v>
       </c>
@@ -25164,7 +25184,7 @@
       </c>
       <c r="O411" s="52"/>
     </row>
-    <row r="412" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A412" s="1" t="s">
         <v>880</v>
       </c>
@@ -25202,7 +25222,7 @@
       </c>
       <c r="O412" s="52"/>
     </row>
-    <row r="413" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A413" s="1" t="s">
         <v>881</v>
       </c>
@@ -25235,7 +25255,7 @@
       <c r="L413" s="145"/>
       <c r="O413" s="52"/>
     </row>
-    <row r="414" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A414" s="1" t="s">
         <v>882</v>
       </c>
@@ -25268,7 +25288,7 @@
       <c r="L414" s="145"/>
       <c r="O414" s="52"/>
     </row>
-    <row r="415" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A415" s="1" t="s">
         <v>883</v>
       </c>
@@ -25301,7 +25321,7 @@
       <c r="L415" s="145"/>
       <c r="O415" s="52"/>
     </row>
-    <row r="416" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A416" s="1" t="s">
         <v>884</v>
       </c>
@@ -25334,7 +25354,7 @@
       <c r="L416" s="145"/>
       <c r="O416" s="52"/>
     </row>
-    <row r="417" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A417" s="1" t="s">
         <v>885</v>
       </c>
@@ -25367,7 +25387,7 @@
       <c r="L417" s="145"/>
       <c r="O417" s="52"/>
     </row>
-    <row r="418" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A418" s="1" t="s">
         <v>886</v>
       </c>
@@ -25405,7 +25425,7 @@
       </c>
       <c r="O418" s="52"/>
     </row>
-    <row r="419" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A419" s="1" t="s">
         <v>887</v>
       </c>
@@ -25438,7 +25458,7 @@
       <c r="L419" s="145"/>
       <c r="O419" s="52"/>
     </row>
-    <row r="420" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A420" s="1" t="s">
         <v>378</v>
       </c>
@@ -25476,7 +25496,7 @@
       </c>
       <c r="O420" s="52"/>
     </row>
-    <row r="421" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A421" s="1" t="s">
         <v>379</v>
       </c>
@@ -25541,7 +25561,7 @@
       </c>
       <c r="K422" s="212">
         <f t="shared" ref="K422:L422" si="235">K423</f>
-        <v>0</v>
+        <v>11680000</v>
       </c>
       <c r="L422" s="212">
         <f t="shared" si="235"/>
@@ -25579,7 +25599,7 @@
       </c>
       <c r="K423" s="151">
         <f t="shared" ref="K423:L423" si="236">SUM(K424,K430)</f>
-        <v>0</v>
+        <v>11680000</v>
       </c>
       <c r="L423" s="151">
         <f t="shared" si="236"/>
@@ -25623,7 +25643,7 @@
       </c>
       <c r="K424" s="148">
         <f t="shared" ref="K424:L424" si="237">SUM(K425:K429)</f>
-        <v>0</v>
+        <v>7100000</v>
       </c>
       <c r="L424" s="148">
         <f t="shared" si="237"/>
@@ -25660,7 +25680,9 @@
         <f t="shared" ref="J425:J429" si="239">G425-I425</f>
         <v>13500000</v>
       </c>
-      <c r="K425" s="145"/>
+      <c r="K425" s="145">
+        <v>1600000</v>
+      </c>
       <c r="L425" s="145"/>
       <c r="O425" s="52"/>
     </row>
@@ -25693,7 +25715,9 @@
         <f t="shared" si="239"/>
         <v>6000000</v>
       </c>
-      <c r="K426" s="145"/>
+      <c r="K426" s="145">
+        <v>1500000</v>
+      </c>
       <c r="L426" s="145"/>
       <c r="O426" s="52"/>
     </row>
@@ -25726,7 +25750,9 @@
         <f t="shared" si="239"/>
         <v>6000000</v>
       </c>
-      <c r="K427" s="145"/>
+      <c r="K427" s="145">
+        <v>1500000</v>
+      </c>
       <c r="L427" s="145"/>
       <c r="O427" s="52"/>
     </row>
@@ -25759,7 +25785,9 @@
         <f t="shared" si="239"/>
         <v>4000000</v>
       </c>
-      <c r="K428" s="145"/>
+      <c r="K428" s="145">
+        <v>1000000</v>
+      </c>
       <c r="L428" s="145"/>
       <c r="O428" s="52"/>
     </row>
@@ -25792,7 +25820,9 @@
         <f t="shared" si="239"/>
         <v>6000000</v>
       </c>
-      <c r="K429" s="145"/>
+      <c r="K429" s="145">
+        <v>1500000</v>
+      </c>
       <c r="L429" s="145"/>
       <c r="O429" s="52"/>
     </row>
@@ -25826,7 +25856,7 @@
       </c>
       <c r="K430" s="148">
         <f t="shared" ref="K430:L430" si="240">K431</f>
-        <v>0</v>
+        <v>4580000</v>
       </c>
       <c r="L430" s="148">
         <f t="shared" si="240"/>
@@ -25863,7 +25893,9 @@
         <f>G431-I431</f>
         <v>68811000</v>
       </c>
-      <c r="K431" s="145"/>
+      <c r="K431" s="145">
+        <v>4580000</v>
+      </c>
       <c r="L431" s="145"/>
       <c r="O431" s="52"/>
     </row>
@@ -25901,7 +25933,7 @@
       </c>
       <c r="K432" s="172">
         <f t="shared" ref="K432:L432" si="241">K433</f>
-        <v>48120000</v>
+        <v>37620000</v>
       </c>
       <c r="L432" s="172">
         <f t="shared" si="241"/>
@@ -25941,7 +25973,7 @@
       </c>
       <c r="K433" s="175">
         <f t="shared" ref="K433:L433" si="242">SUM(K434,K444,K454,K465,K475,K485,K495)</f>
-        <v>48120000</v>
+        <v>37620000</v>
       </c>
       <c r="L433" s="175">
         <f t="shared" si="242"/>
@@ -25979,7 +26011,7 @@
       </c>
       <c r="K434" s="160">
         <f t="shared" ref="K434:L434" si="243">SUM(K435,K440,K442)</f>
-        <v>2500000</v>
+        <v>4000000</v>
       </c>
       <c r="L434" s="160">
         <f t="shared" si="243"/>
@@ -26023,7 +26055,7 @@
       </c>
       <c r="K435" s="154">
         <f t="shared" ref="K435:L435" si="244">SUM(K436:K439)</f>
-        <v>2500000</v>
+        <v>4000000</v>
       </c>
       <c r="L435" s="154">
         <f t="shared" si="244"/>
@@ -26031,7 +26063,7 @@
       </c>
       <c r="O435" s="52"/>
     </row>
-    <row r="436" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A436" s="1" t="s">
         <v>399</v>
       </c>
@@ -26093,7 +26125,9 @@
         <f t="shared" si="246"/>
         <v>6000000</v>
       </c>
-      <c r="K437" s="145"/>
+      <c r="K437" s="145">
+        <v>1500000</v>
+      </c>
       <c r="L437" s="145"/>
       <c r="O437" s="52"/>
     </row>
@@ -26167,7 +26201,7 @@
       <c r="L439" s="145"/>
       <c r="O439" s="52"/>
     </row>
-    <row r="440" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A440" s="1" t="s">
         <v>403</v>
       </c>
@@ -26205,7 +26239,7 @@
       </c>
       <c r="O440" s="52"/>
     </row>
-    <row r="441" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A441" s="1" t="s">
         <v>404</v>
       </c>
@@ -26238,7 +26272,7 @@
       <c r="L441" s="145"/>
       <c r="O441" s="52"/>
     </row>
-    <row r="442" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A442" s="1" t="s">
         <v>894</v>
       </c>
@@ -26276,7 +26310,7 @@
       </c>
       <c r="O442" s="52"/>
     </row>
-    <row r="443" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A443" s="1" t="s">
         <v>895</v>
       </c>
@@ -26339,7 +26373,7 @@
       </c>
       <c r="K444" s="160">
         <f t="shared" ref="K444:L444" si="249">SUM(K445,K450,K452)</f>
-        <v>10700000</v>
+        <v>6700000</v>
       </c>
       <c r="L444" s="160">
         <f t="shared" si="249"/>
@@ -26383,7 +26417,7 @@
       </c>
       <c r="K445" s="154">
         <f t="shared" ref="K445:L445" si="250">SUM(K446:K449)</f>
-        <v>5500000</v>
+        <v>1500000</v>
       </c>
       <c r="L445" s="154">
         <f t="shared" si="250"/>
@@ -26426,7 +26460,7 @@
       <c r="L446" s="145"/>
       <c r="O446" s="52"/>
     </row>
-    <row r="447" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A447" s="1" t="s">
         <v>408</v>
       </c>
@@ -26455,13 +26489,11 @@
         <f t="shared" si="252"/>
         <v>6000000</v>
       </c>
-      <c r="K447" s="145">
-        <v>1500000</v>
-      </c>
+      <c r="K447" s="145"/>
       <c r="L447" s="145"/>
       <c r="O447" s="52"/>
     </row>
-    <row r="448" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A448" s="1" t="s">
         <v>898</v>
       </c>
@@ -26490,13 +26522,11 @@
         <f t="shared" si="252"/>
         <v>6000000</v>
       </c>
-      <c r="K448" s="145">
-        <v>1500000</v>
-      </c>
+      <c r="K448" s="145"/>
       <c r="L448" s="145"/>
       <c r="O448" s="52"/>
     </row>
-    <row r="449" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A449" s="1" t="s">
         <v>899</v>
       </c>
@@ -26525,9 +26555,7 @@
         <f t="shared" si="252"/>
         <v>4000000</v>
       </c>
-      <c r="K449" s="145">
-        <v>1000000</v>
-      </c>
+      <c r="K449" s="145"/>
       <c r="L449" s="145"/>
       <c r="O449" s="52"/>
     </row>
@@ -26604,7 +26632,7 @@
       <c r="L451" s="145"/>
       <c r="O451" s="52"/>
     </row>
-    <row r="452" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A452" s="1" t="s">
         <v>901</v>
       </c>
@@ -26642,7 +26670,7 @@
       </c>
       <c r="O452" s="52"/>
     </row>
-    <row r="453" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A453" s="1" t="s">
         <v>902</v>
       </c>
@@ -26792,7 +26820,7 @@
       <c r="L456" s="145"/>
       <c r="O456" s="52"/>
     </row>
-    <row r="457" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A457" s="1" t="s">
         <v>414</v>
       </c>
@@ -27003,7 +27031,7 @@
       <c r="L462" s="145"/>
       <c r="O462" s="52"/>
     </row>
-    <row r="463" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A463" s="1" t="s">
         <v>913</v>
       </c>
@@ -27041,7 +27069,7 @@
       </c>
       <c r="O463" s="52"/>
     </row>
-    <row r="464" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A464" s="1" t="s">
         <v>914</v>
       </c>
@@ -27104,7 +27132,7 @@
       </c>
       <c r="K465" s="151">
         <f t="shared" ref="K465:L465" si="261">SUM(K466,K471,K473)</f>
-        <v>15200000</v>
+        <v>11200000</v>
       </c>
       <c r="L465" s="151">
         <f t="shared" si="261"/>
@@ -27118,7 +27146,7 @@
       </c>
       <c r="O465" s="52"/>
     </row>
-    <row r="466" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A466" s="1" t="s">
         <v>416</v>
       </c>
@@ -27148,7 +27176,7 @@
       </c>
       <c r="K466" s="148">
         <f t="shared" ref="K466:L466" si="262">SUM(K467:K470)</f>
-        <v>4000000</v>
+        <v>0</v>
       </c>
       <c r="L466" s="148">
         <f t="shared" si="262"/>
@@ -27156,7 +27184,7 @@
       </c>
       <c r="O466" s="52"/>
     </row>
-    <row r="467" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A467" s="94" t="s">
         <v>417</v>
       </c>
@@ -27189,7 +27217,7 @@
       <c r="L467" s="145"/>
       <c r="O467" s="52"/>
     </row>
-    <row r="468" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A468" s="94" t="s">
         <v>418</v>
       </c>
@@ -27218,13 +27246,11 @@
         <f t="shared" si="264"/>
         <v>9000000</v>
       </c>
-      <c r="K468" s="145">
-        <v>1500000</v>
-      </c>
+      <c r="K468" s="145"/>
       <c r="L468" s="145"/>
       <c r="O468" s="52"/>
     </row>
-    <row r="469" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A469" s="94" t="s">
         <v>419</v>
       </c>
@@ -27253,13 +27279,11 @@
         <f t="shared" si="264"/>
         <v>9000000</v>
       </c>
-      <c r="K469" s="145">
-        <v>1500000</v>
-      </c>
+      <c r="K469" s="145"/>
       <c r="L469" s="145"/>
       <c r="O469" s="52"/>
     </row>
-    <row r="470" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A470" s="94" t="s">
         <v>917</v>
       </c>
@@ -27288,9 +27312,7 @@
         <f t="shared" si="264"/>
         <v>6000000</v>
       </c>
-      <c r="K470" s="145">
-        <v>1000000</v>
-      </c>
+      <c r="K470" s="145"/>
       <c r="L470" s="145"/>
       <c r="O470" s="52"/>
     </row>
@@ -27367,7 +27389,7 @@
       <c r="L472" s="145"/>
       <c r="O472" s="52"/>
     </row>
-    <row r="473" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A473" s="1" t="s">
         <v>919</v>
       </c>
@@ -27405,7 +27427,7 @@
       </c>
       <c r="O473" s="52"/>
     </row>
-    <row r="474" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A474" s="1" t="s">
         <v>920</v>
       </c>
@@ -27468,7 +27490,7 @@
       </c>
       <c r="K475" s="160">
         <f t="shared" ref="K475:L475" si="267">SUM(K476,K481,K483)</f>
-        <v>9860000</v>
+        <v>5860000</v>
       </c>
       <c r="L475" s="160">
         <f t="shared" si="267"/>
@@ -27512,7 +27534,7 @@
       </c>
       <c r="K476" s="148">
         <f t="shared" ref="K476:L476" si="268">SUM(K477:K480)</f>
-        <v>4660000</v>
+        <v>660000</v>
       </c>
       <c r="L476" s="148">
         <f t="shared" si="268"/>
@@ -27555,7 +27577,7 @@
       <c r="L477" s="145"/>
       <c r="O477" s="52"/>
     </row>
-    <row r="478" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A478" s="1" t="s">
         <v>425</v>
       </c>
@@ -27584,13 +27606,11 @@
         <f t="shared" si="270"/>
         <v>9000000</v>
       </c>
-      <c r="K478" s="145">
-        <v>1500000</v>
-      </c>
+      <c r="K478" s="145"/>
       <c r="L478" s="145"/>
       <c r="O478" s="52"/>
     </row>
-    <row r="479" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A479" s="1" t="s">
         <v>922</v>
       </c>
@@ -27619,13 +27639,11 @@
         <f t="shared" si="270"/>
         <v>9000000</v>
       </c>
-      <c r="K479" s="145">
-        <v>1500000</v>
-      </c>
+      <c r="K479" s="145"/>
       <c r="L479" s="145"/>
       <c r="O479" s="52"/>
     </row>
-    <row r="480" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A480" s="1" t="s">
         <v>923</v>
       </c>
@@ -27654,9 +27672,7 @@
         <f t="shared" si="270"/>
         <v>6000000</v>
       </c>
-      <c r="K480" s="145">
-        <v>1000000</v>
-      </c>
+      <c r="K480" s="145"/>
       <c r="L480" s="145"/>
       <c r="O480" s="52"/>
     </row>
@@ -27733,7 +27749,7 @@
       <c r="L482" s="145"/>
       <c r="O482" s="52"/>
     </row>
-    <row r="483" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A483" s="1" t="s">
         <v>927</v>
       </c>
@@ -27771,7 +27787,7 @@
       </c>
       <c r="O483" s="52"/>
     </row>
-    <row r="484" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A484" s="1" t="s">
         <v>928</v>
       </c>
@@ -27804,7 +27820,7 @@
       <c r="L484" s="145"/>
       <c r="O484" s="52"/>
     </row>
-    <row r="485" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A485" s="1" t="s">
         <v>426</v>
       </c>
@@ -27848,7 +27864,7 @@
       </c>
       <c r="O485" s="52"/>
     </row>
-    <row r="486" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A486" s="1" t="s">
         <v>428</v>
       </c>
@@ -27886,7 +27902,7 @@
       </c>
       <c r="O486" s="52"/>
     </row>
-    <row r="487" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A487" s="1" t="s">
         <v>429</v>
       </c>
@@ -27919,7 +27935,7 @@
       <c r="L487" s="145"/>
       <c r="O487" s="52"/>
     </row>
-    <row r="488" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A488" s="1" t="s">
         <v>930</v>
       </c>
@@ -27952,7 +27968,7 @@
       <c r="L488" s="145"/>
       <c r="O488" s="52"/>
     </row>
-    <row r="489" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A489" s="1" t="s">
         <v>931</v>
       </c>
@@ -27985,7 +28001,7 @@
       <c r="L489" s="145"/>
       <c r="O489" s="52"/>
     </row>
-    <row r="490" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A490" s="1" t="s">
         <v>932</v>
       </c>
@@ -28018,7 +28034,7 @@
       <c r="L490" s="145"/>
       <c r="O490" s="52"/>
     </row>
-    <row r="491" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A491" s="1" t="s">
         <v>933</v>
       </c>
@@ -28056,7 +28072,7 @@
       </c>
       <c r="O491" s="52"/>
     </row>
-    <row r="492" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A492" s="1" t="s">
         <v>934</v>
       </c>
@@ -28089,7 +28105,7 @@
       <c r="L492" s="145"/>
       <c r="O492" s="52"/>
     </row>
-    <row r="493" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A493" s="1" t="s">
         <v>430</v>
       </c>
@@ -28127,7 +28143,7 @@
       </c>
       <c r="O493" s="52"/>
     </row>
-    <row r="494" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A494" s="1" t="s">
         <v>431</v>
       </c>
@@ -28160,7 +28176,7 @@
       <c r="L494" s="145"/>
       <c r="O494" s="52"/>
     </row>
-    <row r="495" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A495" s="1" t="s">
         <v>432</v>
       </c>
@@ -28204,7 +28220,7 @@
       </c>
       <c r="O495" s="52"/>
     </row>
-    <row r="496" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A496" s="1" t="s">
         <v>936</v>
       </c>
@@ -28242,7 +28258,7 @@
       </c>
       <c r="O496" s="52"/>
     </row>
-    <row r="497" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A497" s="1" t="s">
         <v>937</v>
       </c>
@@ -28275,7 +28291,7 @@
       <c r="L497" s="145"/>
       <c r="O497" s="52"/>
     </row>
-    <row r="498" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A498" s="1" t="s">
         <v>938</v>
       </c>
@@ -28308,7 +28324,7 @@
       <c r="L498" s="145"/>
       <c r="O498" s="52"/>
     </row>
-    <row r="499" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A499" s="1" t="s">
         <v>939</v>
       </c>
@@ -28341,7 +28357,7 @@
       <c r="L499" s="145"/>
       <c r="O499" s="52"/>
     </row>
-    <row r="500" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="500" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A500" s="1" t="s">
         <v>940</v>
       </c>
@@ -28374,7 +28390,7 @@
       <c r="L500" s="145"/>
       <c r="O500" s="52"/>
     </row>
-    <row r="501" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="501" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A501" s="1" t="s">
         <v>941</v>
       </c>
@@ -28412,7 +28428,7 @@
       </c>
       <c r="O501" s="52"/>
     </row>
-    <row r="502" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="502" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A502" s="1" t="s">
         <v>942</v>
       </c>
@@ -28445,7 +28461,7 @@
       <c r="L502" s="145"/>
       <c r="O502" s="52"/>
     </row>
-    <row r="503" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="503" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A503" s="1" t="s">
         <v>943</v>
       </c>
@@ -28483,7 +28499,7 @@
       </c>
       <c r="O503" s="52"/>
     </row>
-    <row r="504" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="504" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A504" s="1" t="s">
         <v>944</v>
       </c>
@@ -28516,7 +28532,7 @@
       <c r="L504" s="145"/>
       <c r="O504" s="52"/>
     </row>
-    <row r="505" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="505" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A505" s="1" t="s">
         <v>433</v>
       </c>
@@ -28554,7 +28570,7 @@
       </c>
       <c r="O505" s="52"/>
     </row>
-    <row r="506" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="506" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A506" s="1" t="s">
         <v>435</v>
       </c>
@@ -28596,7 +28612,7 @@
       </c>
       <c r="O506" s="52"/>
     </row>
-    <row r="507" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="507" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A507" s="1" t="s">
         <v>438</v>
       </c>
@@ -28638,7 +28654,7 @@
       </c>
       <c r="O507" s="52"/>
     </row>
-    <row r="508" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="508" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A508" s="1" t="s">
         <v>441</v>
       </c>
@@ -28678,7 +28694,7 @@
       </c>
       <c r="O508" s="52"/>
     </row>
-    <row r="509" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="509" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A509" s="1" t="s">
         <v>443</v>
       </c>
@@ -28722,7 +28738,7 @@
       </c>
       <c r="O509" s="52"/>
     </row>
-    <row r="510" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="510" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A510" s="1" t="s">
         <v>445</v>
       </c>
@@ -28760,7 +28776,7 @@
       </c>
       <c r="O510" s="52"/>
     </row>
-    <row r="511" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="511" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A511" s="1" t="s">
         <v>446</v>
       </c>
@@ -28793,7 +28809,7 @@
       <c r="L511" s="145"/>
       <c r="O511" s="52"/>
     </row>
-    <row r="512" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="512" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A512" s="1" t="s">
         <v>447</v>
       </c>
@@ -28826,7 +28842,7 @@
       <c r="L512" s="145"/>
       <c r="O512" s="52"/>
     </row>
-    <row r="513" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="513" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A513" s="1" t="s">
         <v>448</v>
       </c>
@@ -28859,7 +28875,7 @@
       <c r="L513" s="145"/>
       <c r="O513" s="52"/>
     </row>
-    <row r="514" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="514" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A514" s="1" t="s">
         <v>449</v>
       </c>
@@ -28892,7 +28908,7 @@
       <c r="L514" s="145"/>
       <c r="O514" s="52"/>
     </row>
-    <row r="515" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="515" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A515" s="1" t="s">
         <v>450</v>
       </c>
@@ -28925,7 +28941,7 @@
       <c r="L515" s="145"/>
       <c r="O515" s="52"/>
     </row>
-    <row r="516" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="516" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A516" s="1" t="s">
         <v>950</v>
       </c>
@@ -28958,7 +28974,7 @@
       <c r="L516" s="145"/>
       <c r="O516" s="52"/>
     </row>
-    <row r="517" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="517" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A517" s="1" t="s">
         <v>451</v>
       </c>
@@ -28996,7 +29012,7 @@
       </c>
       <c r="O517" s="52"/>
     </row>
-    <row r="518" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="518" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A518" s="1" t="s">
         <v>452</v>
       </c>
@@ -29029,7 +29045,7 @@
       <c r="L518" s="145"/>
       <c r="O518" s="52"/>
     </row>
-    <row r="519" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="519" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A519" s="1" t="s">
         <v>453</v>
       </c>
@@ -29062,7 +29078,7 @@
       <c r="L519" s="145"/>
       <c r="O519" s="52"/>
     </row>
-    <row r="520" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="520" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A520" s="1" t="s">
         <v>454</v>
       </c>
@@ -29100,7 +29116,7 @@
       </c>
       <c r="O520" s="52"/>
     </row>
-    <row r="521" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="521" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A521" s="1" t="s">
         <v>455</v>
       </c>
@@ -29133,7 +29149,7 @@
       <c r="L521" s="145"/>
       <c r="O521" s="52"/>
     </row>
-    <row r="522" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="522" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A522" s="1" t="s">
         <v>456</v>
       </c>
@@ -29171,7 +29187,7 @@
       </c>
       <c r="O522" s="52"/>
     </row>
-    <row r="523" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="523" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A523" s="94" t="s">
         <v>457</v>
       </c>
@@ -29204,7 +29220,7 @@
       <c r="L523" s="145"/>
       <c r="O523" s="52"/>
     </row>
-    <row r="524" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="524" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A524" s="1" t="s">
         <v>458</v>
       </c>
@@ -29242,7 +29258,7 @@
       </c>
       <c r="O524" s="52"/>
     </row>
-    <row r="525" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="525" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A525" s="1" t="s">
         <v>459</v>
       </c>
@@ -29275,7 +29291,7 @@
       <c r="L525" s="145"/>
       <c r="O525" s="52"/>
     </row>
-    <row r="526" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="526" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A526" s="1" t="s">
         <v>460</v>
       </c>
@@ -29308,7 +29324,7 @@
       <c r="L526" s="145"/>
       <c r="O526" s="52"/>
     </row>
-    <row r="527" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="527" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A527" s="1" t="s">
         <v>461</v>
       </c>
@@ -29352,7 +29368,7 @@
       </c>
       <c r="O527" s="52"/>
     </row>
-    <row r="528" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="528" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A528" s="1" t="s">
         <v>463</v>
       </c>
@@ -29390,7 +29406,7 @@
       </c>
       <c r="O528" s="52"/>
     </row>
-    <row r="529" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="529" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A529" s="1" t="s">
         <v>464</v>
       </c>
@@ -29423,7 +29439,7 @@
       <c r="L529" s="145"/>
       <c r="O529" s="52"/>
     </row>
-    <row r="530" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="530" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A530" s="1" t="s">
         <v>465</v>
       </c>
@@ -29456,7 +29472,7 @@
       <c r="L530" s="145"/>
       <c r="O530" s="52"/>
     </row>
-    <row r="531" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="531" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A531" s="1" t="s">
         <v>466</v>
       </c>
@@ -29489,7 +29505,7 @@
       <c r="L531" s="145"/>
       <c r="O531" s="52"/>
     </row>
-    <row r="532" spans="1:15" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="532" spans="1:15" ht="15.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A532" s="1" t="s">
         <v>467</v>
       </c>
@@ -29522,7 +29538,7 @@
       <c r="L532" s="145"/>
       <c r="O532" s="52"/>
     </row>
-    <row r="533" spans="1:15" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="533" spans="1:15" ht="15.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A533" s="1" t="s">
         <v>468</v>
       </c>
@@ -29555,7 +29571,7 @@
       <c r="L533" s="145"/>
       <c r="O533" s="52"/>
     </row>
-    <row r="534" spans="1:15" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="534" spans="1:15" ht="15.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A534" s="1" t="s">
         <v>958</v>
       </c>
@@ -29588,7 +29604,7 @@
       <c r="L534" s="145"/>
       <c r="O534" s="52"/>
     </row>
-    <row r="535" spans="1:15" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="535" spans="1:15" ht="15.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A535" s="1" t="s">
         <v>469</v>
       </c>
@@ -29626,7 +29642,7 @@
       </c>
       <c r="O535" s="52"/>
     </row>
-    <row r="536" spans="1:15" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="536" spans="1:15" ht="15.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A536" s="1" t="s">
         <v>470</v>
       </c>
@@ -29659,7 +29675,7 @@
       <c r="L536" s="145"/>
       <c r="O536" s="52"/>
     </row>
-    <row r="537" spans="1:15" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="537" spans="1:15" ht="15.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A537" s="1" t="s">
         <v>471</v>
       </c>
@@ -29692,7 +29708,7 @@
       <c r="L537" s="145"/>
       <c r="O537" s="52"/>
     </row>
-    <row r="538" spans="1:15" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="538" spans="1:15" ht="15.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A538" s="1" t="s">
         <v>472</v>
       </c>
@@ -29730,7 +29746,7 @@
       </c>
       <c r="O538" s="52"/>
     </row>
-    <row r="539" spans="1:15" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="539" spans="1:15" ht="15.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A539" s="1" t="s">
         <v>473</v>
       </c>
@@ -29763,7 +29779,7 @@
       <c r="L539" s="145"/>
       <c r="O539" s="52"/>
     </row>
-    <row r="540" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="540" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A540" s="1" t="s">
         <v>474</v>
       </c>
@@ -29801,7 +29817,7 @@
       </c>
       <c r="O540" s="52"/>
     </row>
-    <row r="541" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="541" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A541" s="1" t="s">
         <v>475</v>
       </c>
@@ -29834,7 +29850,7 @@
       <c r="L541" s="145"/>
       <c r="O541" s="52"/>
     </row>
-    <row r="542" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="542" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A542" s="1" t="s">
         <v>476</v>
       </c>
@@ -29867,7 +29883,7 @@
       <c r="L542" s="145"/>
       <c r="O542" s="52"/>
     </row>
-    <row r="543" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="543" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A543" s="1" t="s">
         <v>477</v>
       </c>
@@ -29905,7 +29921,7 @@
       </c>
       <c r="O543" s="52"/>
     </row>
-    <row r="544" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="544" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A544" s="1" t="s">
         <v>479</v>
       </c>
@@ -29938,7 +29954,7 @@
       <c r="L544" s="145"/>
       <c r="O544" s="52"/>
     </row>
-    <row r="545" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="545" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A545" s="1" t="s">
         <v>481</v>
       </c>
@@ -29971,7 +29987,7 @@
       <c r="L545" s="145"/>
       <c r="O545" s="52"/>
     </row>
-    <row r="546" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="546" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A546" s="1" t="s">
         <v>482</v>
       </c>
@@ -30004,7 +30020,7 @@
       <c r="L546" s="145"/>
       <c r="O546" s="52"/>
     </row>
-    <row r="547" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="547" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A547" s="1" t="s">
         <v>483</v>
       </c>
@@ -30048,7 +30064,7 @@
       </c>
       <c r="O547" s="52"/>
     </row>
-    <row r="548" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="548" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A548" s="1" t="s">
         <v>485</v>
       </c>
@@ -30086,7 +30102,7 @@
       </c>
       <c r="O548" s="52"/>
     </row>
-    <row r="549" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="549" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A549" s="1" t="s">
         <v>486</v>
       </c>
@@ -30119,7 +30135,7 @@
       <c r="L549" s="145"/>
       <c r="O549" s="52"/>
     </row>
-    <row r="550" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="550" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A550" s="1" t="s">
         <v>487</v>
       </c>
@@ -30152,7 +30168,7 @@
       <c r="L550" s="145"/>
       <c r="O550" s="52"/>
     </row>
-    <row r="551" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="551" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A551" s="1" t="s">
         <v>488</v>
       </c>
@@ -30185,7 +30201,7 @@
       <c r="L551" s="145"/>
       <c r="O551" s="52"/>
     </row>
-    <row r="552" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="552" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A552" s="1" t="s">
         <v>489</v>
       </c>
@@ -30223,7 +30239,7 @@
       </c>
       <c r="O552" s="52"/>
     </row>
-    <row r="553" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="553" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A553" s="1" t="s">
         <v>490</v>
       </c>
@@ -30256,7 +30272,7 @@
       <c r="L553" s="145"/>
       <c r="O553" s="52"/>
     </row>
-    <row r="554" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="554" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A554" s="1" t="s">
         <v>491</v>
       </c>
@@ -30294,7 +30310,7 @@
       </c>
       <c r="O554" s="52"/>
     </row>
-    <row r="555" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="555" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A555" s="1" t="s">
         <v>493</v>
       </c>
@@ -30327,7 +30343,7 @@
       <c r="L555" s="145"/>
       <c r="O555" s="52"/>
     </row>
-    <row r="556" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="556" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A556" s="1" t="s">
         <v>494</v>
       </c>
@@ -30367,7 +30383,7 @@
       </c>
       <c r="O556" s="52"/>
     </row>
-    <row r="557" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="557" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A557" s="1" t="s">
         <v>496</v>
       </c>
@@ -30411,7 +30427,7 @@
       </c>
       <c r="O557" s="52"/>
     </row>
-    <row r="558" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="558" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A558" s="1" t="s">
         <v>497</v>
       </c>
@@ -30449,7 +30465,7 @@
       </c>
       <c r="O558" s="52"/>
     </row>
-    <row r="559" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="559" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A559" s="1" t="s">
         <v>498</v>
       </c>
@@ -30482,7 +30498,7 @@
       <c r="L559" s="145"/>
       <c r="O559" s="52"/>
     </row>
-    <row r="560" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="560" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A560" s="1" t="s">
         <v>499</v>
       </c>
@@ -30515,7 +30531,7 @@
       <c r="L560" s="145"/>
       <c r="O560" s="52"/>
     </row>
-    <row r="561" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="561" spans="1:15" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A561" s="1" t="s">
         <v>965</v>
       </c>
@@ -30548,7 +30564,7 @@
       <c r="L561" s="145"/>
       <c r="O561" s="52"/>
     </row>
-    <row r="562" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="562" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A562" s="1" t="s">
         <v>966</v>
       </c>
@@ -30581,7 +30597,7 @@
       <c r="L562" s="145"/>
       <c r="O562" s="52"/>
     </row>
-    <row r="563" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="563" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A563" s="1" t="s">
         <v>967</v>
       </c>
@@ -30619,7 +30635,7 @@
       </c>
       <c r="O563" s="52"/>
     </row>
-    <row r="564" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="564" spans="1:15" ht="13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A564" s="1" t="s">
         <v>968</v>
       </c>
@@ -30666,7 +30682,7 @@
       <c r="D566" s="7"/>
       <c r="F566" s="8"/>
       <c r="G566" s="84" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="I566" s="2"/>
     </row>
@@ -30684,7 +30700,7 @@
       <c r="D568" s="7"/>
       <c r="F568" s="8"/>
       <c r="G568" s="84" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="I568" s="2"/>
     </row>
@@ -30712,7 +30728,7 @@
       </c>
       <c r="I571" s="2"/>
       <c r="J571" s="234" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="572" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -30725,7 +30741,7 @@
       </c>
       <c r="I572" s="2"/>
       <c r="J572" s="234" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="573" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -34264,7 +34280,80 @@
       <c r="I965" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A14:N564" xr:uid="{3A6C5435-28AC-48AD-A4AE-D532A2415063}"/>
+  <autoFilter ref="A14:N564" xr:uid="{3A6C5435-28AC-48AD-A4AE-D532A2415063}">
+    <filterColumn colId="10">
+      <filters>
+        <filter val="1.000.000"/>
+        <filter val="1.200.000"/>
+        <filter val="1.500.000"/>
+        <filter val="1.600.000"/>
+        <filter val="109.590.000"/>
+        <filter val="11.042.000"/>
+        <filter val="11.200.000"/>
+        <filter val="11.687.400"/>
+        <filter val="113.590.000"/>
+        <filter val="12.000.000"/>
+        <filter val="12.240.000"/>
+        <filter val="12.500.000"/>
+        <filter val="13.300.000"/>
+        <filter val="14.292.000"/>
+        <filter val="14.700.000"/>
+        <filter val="143.892.000"/>
+        <filter val="15.100.000"/>
+        <filter val="15.300.000"/>
+        <filter val="16.000.000"/>
+        <filter val="17.050.000"/>
+        <filter val="18.137.400"/>
+        <filter val="18.800.000"/>
+        <filter val="189.347.400"/>
+        <filter val="2.000.000"/>
+        <filter val="2.250.000"/>
+        <filter val="2.500.000"/>
+        <filter val="20.000.000"/>
+        <filter val="24.300.000"/>
+        <filter val="250.000"/>
+        <filter val="29.800.000"/>
+        <filter val="3.000.000"/>
+        <filter val="3.250.000"/>
+        <filter val="3.500.000"/>
+        <filter val="30.000.000"/>
+        <filter val="30.292.000"/>
+        <filter val="300.000"/>
+        <filter val="33.300.000"/>
+        <filter val="333.239.400"/>
+        <filter val="36.540.000"/>
+        <filter val="37.620.000"/>
+        <filter val="39.040.000"/>
+        <filter val="4.000.000"/>
+        <filter val="4.500.000"/>
+        <filter val="4.587.400"/>
+        <filter val="4.660.000"/>
+        <filter val="4.750.000"/>
+        <filter val="41.300.000"/>
+        <filter val="42.500.000"/>
+        <filter val="5.000.000"/>
+        <filter val="5.100.000"/>
+        <filter val="5.200.000"/>
+        <filter val="5.250.000"/>
+        <filter val="5.860.000"/>
+        <filter val="6.000.000"/>
+        <filter val="6.450.000"/>
+        <filter val="6.700.000"/>
+        <filter val="600.000"/>
+        <filter val="660.000"/>
+        <filter val="7.100.000"/>
+        <filter val="75.757.400"/>
+        <filter val="750.000"/>
+        <filter val="8.000.000"/>
+        <filter val="8.250.000"/>
+        <filter val="8.700.000"/>
+        <filter val="9.000.000"/>
+        <filter val="9.550.000"/>
+        <filter val="9.600.000"/>
+        <filter val="9.860.000"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="4">
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="E112:F112"/>
@@ -34341,7 +34430,7 @@
   </sheetPr>
   <dimension ref="B2:XEW997"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
@@ -34361,17 +34450,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16377" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="256" t="s">
-        <v>973</v>
-      </c>
-      <c r="C2" s="256"/>
-      <c r="D2" s="256"/>
-      <c r="E2" s="256"/>
-      <c r="F2" s="256"/>
-      <c r="G2" s="256"/>
-      <c r="H2" s="256"/>
-      <c r="I2" s="256"/>
-      <c r="J2" s="256"/>
+      <c r="B2" s="248" t="s">
+        <v>972</v>
+      </c>
+      <c r="C2" s="248"/>
+      <c r="D2" s="248"/>
+      <c r="E2" s="248"/>
+      <c r="F2" s="248"/>
+      <c r="G2" s="248"/>
+      <c r="H2" s="248"/>
+      <c r="I2" s="248"/>
+      <c r="J2" s="248"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
@@ -50741,17 +50830,17 @@
       <c r="XEW2" s="3"/>
     </row>
     <row r="3" spans="2:16377" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="257" t="s">
+      <c r="B3" s="249" t="s">
         <v>521</v>
       </c>
-      <c r="C3" s="257"/>
-      <c r="D3" s="257"/>
-      <c r="E3" s="257"/>
-      <c r="F3" s="257"/>
-      <c r="G3" s="257"/>
-      <c r="H3" s="257"/>
-      <c r="I3" s="257"/>
-      <c r="J3" s="257"/>
+      <c r="C3" s="249"/>
+      <c r="D3" s="249"/>
+      <c r="E3" s="249"/>
+      <c r="F3" s="249"/>
+      <c r="G3" s="249"/>
+      <c r="H3" s="249"/>
+      <c r="I3" s="249"/>
+      <c r="J3" s="249"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -67122,42 +67211,42 @@
     </row>
     <row r="4" spans="2:16377" ht="15.5" x14ac:dyDescent="0.35"/>
     <row r="5" spans="2:16377" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="258" t="s">
+      <c r="B5" s="250" t="s">
         <v>522</v>
       </c>
-      <c r="C5" s="259"/>
+      <c r="C5" s="251"/>
       <c r="D5" s="20" t="s">
         <v>523</v>
       </c>
     </row>
     <row r="6" spans="2:16377" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="260" t="s">
+      <c r="B6" s="252" t="s">
         <v>524</v>
       </c>
-      <c r="C6" s="261" t="s">
+      <c r="C6" s="253" t="s">
         <v>525</v>
       </c>
-      <c r="D6" s="261" t="s">
+      <c r="D6" s="253" t="s">
         <v>526</v>
       </c>
-      <c r="E6" s="262" t="str">
+      <c r="E6" s="255" t="str">
         <f>"Pagu "</f>
         <v xml:space="preserve">Pagu </v>
       </c>
-      <c r="F6" s="263" t="s">
+      <c r="F6" s="257" t="s">
         <v>520</v>
       </c>
-      <c r="G6" s="265" t="s">
+      <c r="G6" s="259" t="s">
+        <v>973</v>
+      </c>
+      <c r="H6" s="261" t="s">
         <v>974</v>
       </c>
-      <c r="H6" s="267" t="s">
+      <c r="I6" s="263" t="s">
         <v>975</v>
       </c>
-      <c r="I6" s="269" t="s">
+      <c r="J6" s="265" t="s">
         <v>976</v>
-      </c>
-      <c r="J6" s="271" t="s">
-        <v>977</v>
       </c>
       <c r="K6" s="21"/>
       <c r="L6" s="21"/>
@@ -67166,15 +67255,15 @@
       <c r="O6" s="21"/>
     </row>
     <row r="7" spans="2:16377" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="251"/>
-      <c r="C7" s="248"/>
-      <c r="D7" s="248"/>
-      <c r="E7" s="247"/>
-      <c r="F7" s="264"/>
-      <c r="G7" s="266"/>
-      <c r="H7" s="268"/>
-      <c r="I7" s="270"/>
-      <c r="J7" s="272"/>
+      <c r="B7" s="247"/>
+      <c r="C7" s="254"/>
+      <c r="D7" s="254"/>
+      <c r="E7" s="256"/>
+      <c r="F7" s="258"/>
+      <c r="G7" s="260"/>
+      <c r="H7" s="262"/>
+      <c r="I7" s="264"/>
+      <c r="J7" s="266"/>
       <c r="K7" s="21"/>
       <c r="L7" s="21"/>
       <c r="M7" s="21"/>
@@ -67185,10 +67274,10 @@
       <c r="B8" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="253" t="s">
+      <c r="C8" s="243" t="s">
         <v>527</v>
       </c>
-      <c r="D8" s="254"/>
+      <c r="D8" s="244"/>
       <c r="E8" s="23"/>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -67202,10 +67291,10 @@
       <c r="O8" s="25"/>
     </row>
     <row r="9" spans="2:16377" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="255">
+      <c r="B9" s="245">
         <v>1</v>
       </c>
-      <c r="C9" s="246" t="s">
+      <c r="C9" s="270" t="s">
         <v>500</v>
       </c>
       <c r="D9" s="26" t="s">
@@ -67239,8 +67328,8 @@
       <c r="O9" s="31"/>
     </row>
     <row r="10" spans="2:16377" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="250"/>
-      <c r="C10" s="247"/>
+      <c r="B10" s="246"/>
+      <c r="C10" s="256"/>
       <c r="D10" s="32" t="s">
         <v>502</v>
       </c>
@@ -67254,7 +67343,7 @@
       </c>
       <c r="G10" s="28" cm="1">
         <f t="array" ref="G10">SUM(_xlfn._xlws.FILTER('Usulan TUP 1'!$K$15:$K$564,'Usulan TUP 1'!$N$15:$N$564=D10,0))</f>
-        <v>32542000</v>
+        <v>32540000</v>
       </c>
       <c r="H10" s="28" cm="1">
         <f t="array" ref="H10">SUM(_xlfn._xlws.FILTER('Usulan TUP 1'!$L$15:$L$564,'Usulan TUP 1'!$N$15:$N$564=D10,0))</f>
@@ -67272,8 +67361,8 @@
       <c r="O10" s="31"/>
     </row>
     <row r="11" spans="2:16377" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="251"/>
-      <c r="C11" s="248"/>
+      <c r="B11" s="247"/>
+      <c r="C11" s="254"/>
       <c r="D11" s="76" t="s">
         <v>528</v>
       </c>
@@ -67287,7 +67376,7 @@
       </c>
       <c r="G11" s="78">
         <f t="shared" si="0"/>
-        <v>81142000</v>
+        <v>81140000</v>
       </c>
       <c r="H11" s="78">
         <f t="shared" si="0"/>
@@ -67308,10 +67397,10 @@
       <c r="O11" s="31"/>
     </row>
     <row r="12" spans="2:16377" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="249">
+      <c r="B12" s="271">
         <v>2</v>
       </c>
-      <c r="C12" s="246" t="s">
+      <c r="C12" s="270" t="s">
         <v>508</v>
       </c>
       <c r="D12" s="33" t="s">
@@ -67345,8 +67434,8 @@
       <c r="O12" s="31"/>
     </row>
     <row r="13" spans="2:16377" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="250"/>
-      <c r="C13" s="247"/>
+      <c r="B13" s="246"/>
+      <c r="C13" s="256"/>
       <c r="D13" s="33" t="s">
         <v>510</v>
       </c>
@@ -67360,7 +67449,7 @@
       </c>
       <c r="G13" s="28" cm="1">
         <f t="array" ref="G13">SUM(_xlfn._xlws.FILTER('Usulan TUP 1'!$K$15:$K$564,'Usulan TUP 1'!$N$15:$N$564=D13,0))</f>
-        <v>0</v>
+        <v>18130000</v>
       </c>
       <c r="H13" s="28" cm="1">
         <f t="array" ref="H13">SUM(_xlfn._xlws.FILTER('Usulan TUP 1'!$L$15:$L$564,'Usulan TUP 1'!$N$15:$N$564=D13,0))</f>
@@ -67381,8 +67470,8 @@
       <c r="O13" s="31"/>
     </row>
     <row r="14" spans="2:16377" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="251"/>
-      <c r="C14" s="248"/>
+      <c r="B14" s="247"/>
+      <c r="C14" s="254"/>
       <c r="D14" s="76" t="s">
         <v>529</v>
       </c>
@@ -67396,7 +67485,7 @@
       </c>
       <c r="G14" s="78">
         <f t="shared" si="1"/>
-        <v>24000000</v>
+        <v>42130000</v>
       </c>
       <c r="H14" s="78">
         <f t="shared" si="1"/>
@@ -67417,10 +67506,10 @@
       <c r="O14" s="31"/>
     </row>
     <row r="15" spans="2:16377" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="249">
+      <c r="B15" s="271">
         <v>3</v>
       </c>
-      <c r="C15" s="246" t="s">
+      <c r="C15" s="270" t="s">
         <v>503</v>
       </c>
       <c r="D15" s="33" t="s">
@@ -67454,8 +67543,8 @@
       <c r="O15" s="31"/>
     </row>
     <row r="16" spans="2:16377" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="250"/>
-      <c r="C16" s="247"/>
+      <c r="B16" s="246"/>
+      <c r="C16" s="256"/>
       <c r="D16" s="33" t="s">
         <v>505</v>
       </c>
@@ -67487,8 +67576,8 @@
       <c r="O16" s="31"/>
     </row>
     <row r="17" spans="2:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="251"/>
-      <c r="C17" s="248"/>
+      <c r="B17" s="247"/>
+      <c r="C17" s="254"/>
       <c r="D17" s="76" t="s">
         <v>530</v>
       </c>
@@ -67523,10 +67612,10 @@
       <c r="O17" s="31"/>
     </row>
     <row r="18" spans="2:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="249">
+      <c r="B18" s="271">
         <v>4</v>
       </c>
-      <c r="C18" s="246" t="s">
+      <c r="C18" s="270" t="s">
         <v>506</v>
       </c>
       <c r="D18" s="33" t="s">
@@ -67563,8 +67652,8 @@
       <c r="O18" s="31"/>
     </row>
     <row r="19" spans="2:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="250"/>
-      <c r="C19" s="247"/>
+      <c r="B19" s="246"/>
+      <c r="C19" s="256"/>
       <c r="D19" s="98" t="s">
         <v>511</v>
       </c>
@@ -67578,7 +67667,7 @@
       </c>
       <c r="G19" s="100" cm="1">
         <f t="array" ref="G19">SUM(_xlfn._xlws.FILTER('Usulan TUP 1'!$K$15:$K$564,'Usulan TUP 1'!$N$15:$N$564=D19,0))</f>
-        <v>48120000</v>
+        <v>37620000</v>
       </c>
       <c r="H19" s="100" cm="1">
         <f t="array" ref="H19">SUM(_xlfn._xlws.FILTER('Usulan TUP 1'!$L$15:$L$564,'Usulan TUP 1'!$N$15:$N$564=D19,0))</f>
@@ -67599,8 +67688,8 @@
       <c r="O19" s="31"/>
     </row>
     <row r="20" spans="2:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="251"/>
-      <c r="C20" s="252"/>
+      <c r="B20" s="247"/>
+      <c r="C20" s="272"/>
       <c r="D20" s="222" t="s">
         <v>531</v>
       </c>
@@ -67614,7 +67703,7 @@
       </c>
       <c r="G20" s="224">
         <f>SUM(G18:G19)</f>
-        <v>136660000</v>
+        <v>126160000</v>
       </c>
       <c r="H20" s="224">
         <f t="shared" ref="H20:J20" si="4">SUM(H18:H19)</f>
@@ -67635,11 +67724,11 @@
       <c r="O20" s="31"/>
     </row>
     <row r="21" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="243" t="s">
+      <c r="B21" s="267" t="s">
         <v>532</v>
       </c>
-      <c r="C21" s="244"/>
-      <c r="D21" s="245"/>
+      <c r="C21" s="268"/>
+      <c r="D21" s="269"/>
       <c r="E21" s="233">
         <f>SUM(E11,E14,E17,E20)</f>
         <v>23288180000</v>
@@ -67650,7 +67739,7 @@
       </c>
       <c r="G21" s="233">
         <f t="shared" si="5"/>
-        <v>325602000</v>
+        <v>333230000</v>
       </c>
       <c r="H21" s="226">
         <f t="shared" si="5"/>
@@ -68679,6 +68768,14 @@
     <row r="997" ht="15.5" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="B9:B11"/>
     <mergeCell ref="B2:J2"/>
@@ -68693,18 +68790,10 @@
     <mergeCell ref="H6:H7"/>
     <mergeCell ref="I6:I7"/>
     <mergeCell ref="J6:J7"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C12:C14"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.59055118110236227" right="0.59055118110236227" top="0.74803149606299213" bottom="0.74803149606299213" header="0" footer="0.39370078740157483"/>
-  <pageSetup paperSize="9" scale="63" fitToHeight="0" pageOrder="overThenDown" orientation="portrait" cellComments="atEnd" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="76" fitToHeight="0" pageOrder="overThenDown" orientation="portrait" cellComments="atEnd" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>

</xml_diff>

<commit_message>
Perbaikan Realisasi SP2D 1 Maret 2023
</commit_message>
<xml_diff>
--- a/TUP/TUP 1/Usulan TUP 1.xlsx
+++ b/TUP/TUP 1/Usulan TUP 1.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
-  <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1" defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BACK\PUSDIK\2023\Github\TA.2023\TUP\TUP 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A49C72E-30DF-44B8-AF85-FA06F607D7F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{826DB08B-9BA1-474A-9C77-BEFBBB5C80F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2544" yWindow="2544" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{E899FA34-6DE3-4640-B916-AC504F664995}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E899FA34-6DE3-4640-B916-AC504F664995}"/>
   </bookViews>
   <sheets>
     <sheet name="Rekap TUP 1 Per Akun" sheetId="3" r:id="rId1"/>
@@ -154,7 +154,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="9" r:id="rId9"/>
+    <pivotCache cacheId="0" r:id="rId9"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -3139,9 +3139,6 @@
     <t>Usulan TUP 1</t>
   </si>
   <si>
-    <t>Prediksi Realisasi TUP 1</t>
-  </si>
-  <si>
     <t>Sisa TUP 1
 (Pengembalian)</t>
   </si>
@@ -3202,6 +3199,9 @@
   </si>
   <si>
     <t>Sisa TUP 1</t>
+  </si>
+  <si>
+    <t>Realisasi TUP 1</t>
   </si>
 </sst>
 </file>
@@ -4928,6 +4928,12 @@
     <xf numFmtId="164" fontId="5" fillId="18" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="18" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="22" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4952,26 +4958,6 @@
     <xf numFmtId="0" fontId="9" fillId="40" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="41" fontId="12" fillId="10" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="12" fillId="10" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="12" fillId="10" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -4979,6 +4965,8 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4995,9 +4983,11 @@
     <xf numFmtId="0" fontId="12" fillId="10" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5024,12 +5014,22 @@
     <xf numFmtId="0" fontId="15" fillId="9" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="18" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="12" fillId="10" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="12" fillId="10" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="12" fillId="10" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="22" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
@@ -5902,7 +5902,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$H$34:$H$35" spid="_x0000_s3409"/>
+                  <a14:cameraTool cellRange="$H$34:$H$35" spid="_x0000_s3412"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -8511,7 +8511,7 @@
       <sheetName val="SPP GUP TUP dan LS"/>
       <sheetName val="Pvt Draft SPBy"/>
       <sheetName val="SPBY"/>
-      <sheetName val="Rekap GUP dan TUP"/>
+      <sheetName val="Rekap Gup dan TUP"/>
       <sheetName val="Rincian No SPBy"/>
       <sheetName val="DBSPBY"/>
       <sheetName val="IKU Subkomp"/>
@@ -8519,17 +8519,17 @@
       <sheetName val="Sheet3"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
       <sheetData sheetId="4"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -8644,7 +8644,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1127F9CD-6ADB-4CE5-B7BF-433D4F60FD7D}" name="PivotTable10" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1127F9CD-6ADB-4CE5-B7BF-433D4F60FD7D}" name="PivotTable10" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A11:D25" firstHeaderRow="0" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField name="Program, Kegiatan dan KRO" axis="axisRow" compact="0" outline="0" showAll="0">
@@ -9892,11 +9892,11 @@
       <c r="E4" s="50"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="292" t="s">
-        <v>973</v>
-      </c>
-      <c r="B9" s="292"/>
-      <c r="C9" s="292"/>
+      <c r="A9" s="294" t="s">
+        <v>972</v>
+      </c>
+      <c r="B9" s="294"/>
+      <c r="C9" s="294"/>
       <c r="D9" s="49"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -9924,7 +9924,7 @@
         <v>536</v>
       </c>
       <c r="D11" s="226" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="K11" s="3" t="str" cm="1">
         <f t="array" ref="K11:L20">_xlfn.UNIQUE(MID(_xlfn._xlws.FILTER('Usulan TUP 1'!$A$15:$B$564,(LEN('Usulan TUP 1'!$B$15:$B$564)=6)*('Usulan TUP 1'!$K$15:$K$564&gt;0),""),1,11))</f>
@@ -10277,7 +10277,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="207" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="B24" s="208"/>
       <c r="C24" s="209">
@@ -10412,8 +10412,8 @@
   </sheetPr>
   <dimension ref="A1:R965"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A433" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -10459,7 +10459,7 @@
         <v>513</v>
       </c>
       <c r="G2" s="39" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="I2" s="16"/>
       <c r="J2" s="16"/>
@@ -10478,7 +10478,7 @@
         <v>514</v>
       </c>
       <c r="G3" s="39" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="I3" s="16"/>
       <c r="J3" s="16"/>
@@ -10507,7 +10507,7 @@
     <row r="5" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="B5" s="77" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="C5" s="41"/>
       <c r="D5" s="41"/>
@@ -10641,7 +10641,7 @@
     <row r="11" spans="1:18" s="39" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
       <c r="B11" s="40" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="C11" s="45" t="str">
         <f>": Rp. "&amp;TEXT(K15,"#.##")</f>
@@ -10666,7 +10666,7 @@
     <row r="12" spans="1:18" s="223" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="55"/>
       <c r="B12" s="76" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="C12" s="222" t="str">
         <f>": Rp. "&amp;TEXT(L15,"#.##")</f>
@@ -10708,19 +10708,19 @@
         <v>968</v>
       </c>
       <c r="J13" s="236" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="K13" s="291" t="s">
         <v>967</v>
       </c>
       <c r="L13" s="291" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="M13" s="291" t="s">
+        <v>987</v>
+      </c>
+      <c r="N13" s="292" t="s">
         <v>988</v>
-      </c>
-      <c r="N13" s="330" t="s">
-        <v>989</v>
       </c>
       <c r="O13" s="266" t="s">
         <v>550</v>
@@ -10763,10 +10763,10 @@
       <c r="L14" s="286">
         <v>5</v>
       </c>
-      <c r="M14" s="331">
+      <c r="M14" s="293">
         <v>6</v>
       </c>
-      <c r="N14" s="331">
+      <c r="N14" s="293">
         <v>7</v>
       </c>
       <c r="O14" s="65">
@@ -10812,11 +10812,11 @@
       </c>
       <c r="M15" s="290">
         <f t="shared" si="1"/>
-        <v>182886064</v>
+        <v>198046564</v>
       </c>
       <c r="N15" s="290">
         <f t="shared" si="1"/>
-        <v>84243936</v>
+        <v>69083436</v>
       </c>
       <c r="Q15" s="52"/>
     </row>
@@ -10858,11 +10858,11 @@
       </c>
       <c r="M16" s="95">
         <f t="shared" si="3"/>
-        <v>69925980</v>
+        <v>85086480</v>
       </c>
       <c r="N16" s="95">
         <f t="shared" si="3"/>
-        <v>33824020</v>
+        <v>18663520</v>
       </c>
       <c r="Q16" s="52"/>
     </row>
@@ -10904,11 +10904,11 @@
       </c>
       <c r="M17" s="98">
         <f t="shared" si="3"/>
-        <v>69925980</v>
+        <v>85086480</v>
       </c>
       <c r="N17" s="98">
         <f t="shared" si="3"/>
-        <v>33824020</v>
+        <v>18663520</v>
       </c>
       <c r="Q17" s="52"/>
     </row>
@@ -10925,10 +10925,10 @@
       <c r="D18" s="261">
         <v>5</v>
       </c>
-      <c r="E18" s="293" t="s">
+      <c r="E18" s="295" t="s">
         <v>573</v>
       </c>
-      <c r="F18" s="294"/>
+      <c r="F18" s="296"/>
       <c r="G18" s="101">
         <f>G19</f>
         <v>1000000000</v>
@@ -10954,11 +10954,11 @@
       </c>
       <c r="M18" s="101">
         <f t="shared" si="3"/>
-        <v>69925980</v>
+        <v>85086480</v>
       </c>
       <c r="N18" s="101">
         <f t="shared" si="3"/>
-        <v>33824020</v>
+        <v>18663520</v>
       </c>
       <c r="Q18" s="52"/>
     </row>
@@ -11004,11 +11004,11 @@
       </c>
       <c r="M19" s="104">
         <f t="shared" si="5"/>
-        <v>69925980</v>
+        <v>85086480</v>
       </c>
       <c r="N19" s="104">
         <f t="shared" si="5"/>
-        <v>33824020</v>
+        <v>18663520</v>
       </c>
       <c r="Q19" s="52"/>
     </row>
@@ -11145,7 +11145,7 @@
         <v>4000000</v>
       </c>
       <c r="L22" s="113">
-        <f t="shared" ref="L22:N22" si="11">SUM(L23:L26)</f>
+        <f t="shared" ref="L22" si="11">SUM(L23:L26)</f>
         <v>4000000</v>
       </c>
       <c r="M22" s="113" cm="1">
@@ -11339,7 +11339,7 @@
         <v>16000000</v>
       </c>
       <c r="K27" s="113">
-        <f t="shared" ref="K27:N27" si="14">K28</f>
+        <f t="shared" ref="K27:L27" si="14">K28</f>
         <v>6000000</v>
       </c>
       <c r="L27" s="113">
@@ -11424,7 +11424,7 @@
         <v>67448000</v>
       </c>
       <c r="K29" s="113">
-        <f t="shared" ref="K29:N29" si="15">K30</f>
+        <f t="shared" ref="K29:L29" si="15">K30</f>
         <v>5100000</v>
       </c>
       <c r="L29" s="113">
@@ -11565,7 +11565,7 @@
         <v>4000000</v>
       </c>
       <c r="L32" s="113">
-        <f t="shared" ref="L32:N32" si="19">SUM(L33:L36)</f>
+        <f t="shared" ref="L32" si="19">SUM(L33:L36)</f>
         <v>4000000</v>
       </c>
       <c r="M32" s="113" cm="1">
@@ -11759,7 +11759,7 @@
         <v>5000000</v>
       </c>
       <c r="K37" s="113">
-        <f t="shared" ref="K37:N37" si="22">K38</f>
+        <f t="shared" ref="K37:L37" si="22">K38</f>
         <v>2000000</v>
       </c>
       <c r="L37" s="113">
@@ -11844,7 +11844,7 @@
         <v>32019000</v>
       </c>
       <c r="K39" s="113">
-        <f t="shared" ref="K39:N39" si="23">K40</f>
+        <f t="shared" ref="K39:L39" si="23">K40</f>
         <v>8700000</v>
       </c>
       <c r="L39" s="113">
@@ -12033,7 +12033,7 @@
         <v>4000000</v>
       </c>
       <c r="L43" s="113">
-        <f t="shared" ref="L43:N43" si="29">SUM(L44:L47)</f>
+        <f t="shared" ref="L43" si="29">SUM(L44:L47)</f>
         <v>4000000</v>
       </c>
       <c r="M43" s="113" cm="1">
@@ -12227,7 +12227,7 @@
         <v>24000000</v>
       </c>
       <c r="K48" s="119">
-        <f t="shared" ref="K48:N48" si="32">K49</f>
+        <f t="shared" ref="K48:L48" si="32">K49</f>
         <v>12000000</v>
       </c>
       <c r="L48" s="119">
@@ -12369,7 +12369,7 @@
         <v>3250000</v>
       </c>
       <c r="L51" s="119">
-        <f t="shared" ref="L51:N51" si="36">SUM(L52:L55)</f>
+        <f t="shared" ref="L51" si="36">SUM(L52:L55)</f>
         <v>3250000</v>
       </c>
       <c r="M51" s="113" cm="1">
@@ -12563,7 +12563,7 @@
         <v>4000000</v>
       </c>
       <c r="K56" s="125">
-        <f t="shared" ref="K56:N56" si="39">K57</f>
+        <f t="shared" ref="K56:L56" si="39">K57</f>
         <v>0</v>
       </c>
       <c r="L56" s="125">
@@ -12644,7 +12644,7 @@
         <v>66252000</v>
       </c>
       <c r="K58" s="119">
-        <f t="shared" ref="K58:N58" si="40">K59</f>
+        <f t="shared" ref="K58:L58" si="40">K59</f>
         <v>11040000</v>
       </c>
       <c r="L58" s="119">
@@ -12833,7 +12833,7 @@
         <v>12500000</v>
       </c>
       <c r="L62" s="119">
-        <f t="shared" ref="L62:N62" si="46">SUM(L63:L67)</f>
+        <f t="shared" ref="L62" si="46">SUM(L63:L67)</f>
         <v>12500000</v>
       </c>
       <c r="M62" s="113" cm="1">
@@ -13066,7 +13066,7 @@
         <v>25200000</v>
       </c>
       <c r="K68" s="119">
-        <f t="shared" ref="K68:N68" si="49">K69</f>
+        <f t="shared" ref="K68:L68" si="49">K69</f>
         <v>0</v>
       </c>
       <c r="L68" s="119">
@@ -13147,7 +13147,7 @@
         <v>304120000</v>
       </c>
       <c r="K70" s="119">
-        <f t="shared" ref="K70:N70" si="50">K71</f>
+        <f t="shared" ref="K70:L70" si="50">K71</f>
         <v>30000000</v>
       </c>
       <c r="L70" s="119">
@@ -13232,7 +13232,7 @@
         <v>1500000</v>
       </c>
       <c r="K72" s="119">
-        <f t="shared" ref="K72:N72" si="51">K73</f>
+        <f t="shared" ref="K72:L72" si="51">K73</f>
         <v>0</v>
       </c>
       <c r="L72" s="119">
@@ -13369,7 +13369,7 @@
         <v>0</v>
       </c>
       <c r="L75" s="119">
-        <f t="shared" ref="L75:N75" si="55">SUM(L76:L79)</f>
+        <f t="shared" ref="L75" si="55">SUM(L76:L79)</f>
         <v>0</v>
       </c>
       <c r="M75" s="113" cm="1">
@@ -13551,7 +13551,7 @@
         <v>7200000</v>
       </c>
       <c r="K80" s="113">
-        <f t="shared" ref="K80:N80" si="58">K81</f>
+        <f t="shared" ref="K80:L80" si="58">K81</f>
         <v>0</v>
       </c>
       <c r="L80" s="113">
@@ -13632,7 +13632,7 @@
         <v>40691000</v>
       </c>
       <c r="K82" s="119">
-        <f t="shared" ref="K82:N82" si="59">K83</f>
+        <f t="shared" ref="K82:L82" si="59">K83</f>
         <v>0</v>
       </c>
       <c r="L82" s="119">
@@ -13724,11 +13724,11 @@
       </c>
       <c r="M84" s="128">
         <f t="shared" si="61"/>
-        <v>11702000</v>
+        <v>26862500</v>
       </c>
       <c r="N84" s="128">
         <f t="shared" si="61"/>
-        <v>15948000</v>
+        <v>787500</v>
       </c>
       <c r="Q84" s="52"/>
     </row>
@@ -13817,7 +13817,7 @@
         <v>0</v>
       </c>
       <c r="L86" s="119">
-        <f t="shared" ref="L86:N86" si="65">SUM(L87:L90)</f>
+        <f t="shared" ref="L86" si="65">SUM(L87:L90)</f>
         <v>0</v>
       </c>
       <c r="M86" s="113" cm="1">
@@ -13999,7 +13999,7 @@
         <v>66000000</v>
       </c>
       <c r="K91" s="119">
-        <f t="shared" ref="K91:N91" si="68">K92</f>
+        <f t="shared" ref="K91:L91" si="68">K92</f>
         <v>0</v>
       </c>
       <c r="L91" s="119">
@@ -14089,11 +14089,11 @@
       </c>
       <c r="M93" s="131">
         <f t="shared" si="70"/>
-        <v>11042000</v>
+        <v>26202500</v>
       </c>
       <c r="N93" s="131">
         <f t="shared" si="70"/>
-        <v>16608000</v>
+        <v>1447500</v>
       </c>
       <c r="O93" s="5" t="s">
         <v>503</v>
@@ -14136,7 +14136,7 @@
         <v>8000000</v>
       </c>
       <c r="L94" s="119">
-        <f t="shared" ref="L94:N94" si="72">SUM(L95:L99)</f>
+        <f t="shared" ref="L94" si="72">SUM(L95:L99)</f>
         <v>8000000</v>
       </c>
       <c r="M94" s="113" cm="1">
@@ -14365,7 +14365,7 @@
         <v>10000000</v>
       </c>
       <c r="K100" s="125">
-        <f t="shared" ref="K100:N100" si="75">K101</f>
+        <f t="shared" ref="K100:L100" si="75">K101</f>
         <v>0</v>
       </c>
       <c r="L100" s="125">
@@ -14446,7 +14446,7 @@
         <v>69170000</v>
       </c>
       <c r="K102" s="119">
-        <f t="shared" ref="K102:N102" si="76">K103</f>
+        <f t="shared" ref="K102:L102" si="76">K103</f>
         <v>33300000</v>
       </c>
       <c r="L102" s="119">
@@ -14455,11 +14455,11 @@
       </c>
       <c r="M102" s="113" cm="1">
         <f t="array" ref="M102">SUM(_xlfn._xlws.FILTER([5]!Draft_SPBY[Jumlah],[5]!Draft_SPBY[MAK4]=A102,0))</f>
-        <v>11042000</v>
+        <v>26202500</v>
       </c>
       <c r="N102" s="113">
         <f>L102-M102</f>
-        <v>8608000</v>
+        <v>-6552500</v>
       </c>
       <c r="Q102" s="52"/>
     </row>
@@ -14888,10 +14888,10 @@
       <c r="D112" s="273">
         <v>8</v>
       </c>
-      <c r="E112" s="295" t="s">
+      <c r="E112" s="297" t="s">
         <v>631</v>
       </c>
-      <c r="F112" s="296"/>
+      <c r="F112" s="298"/>
       <c r="G112" s="149">
         <f>SUM(G113,G128,G221)</f>
         <v>10694573000</v>
@@ -15108,7 +15108,7 @@
         <v>4000000</v>
       </c>
       <c r="L116" s="161">
-        <f t="shared" ref="L116:N116" si="89">SUM(L117:L120)</f>
+        <f t="shared" ref="L116" si="89">SUM(L117:L120)</f>
         <v>4000000</v>
       </c>
       <c r="M116" s="113" cm="1">
@@ -15306,7 +15306,7 @@
         <v>0</v>
       </c>
       <c r="L121" s="113">
-        <f t="shared" ref="L121:N121" si="93">SUM(L122:L123)</f>
+        <f t="shared" ref="L121" si="93">SUM(L122:L123)</f>
         <v>0</v>
       </c>
       <c r="M121" s="113" cm="1">
@@ -15418,7 +15418,7 @@
         <v>8000000</v>
       </c>
       <c r="K124" s="164">
-        <f t="shared" ref="K124:N124" si="96">K125</f>
+        <f t="shared" ref="K124:L124" si="96">K125</f>
         <v>0</v>
       </c>
       <c r="L124" s="164">
@@ -15499,7 +15499,7 @@
         <v>197780000</v>
       </c>
       <c r="K126" s="125">
-        <f t="shared" ref="K126:N126" si="97">K127</f>
+        <f t="shared" ref="K126:L126" si="97">K127</f>
         <v>0</v>
       </c>
       <c r="L126" s="125">
@@ -15734,7 +15734,7 @@
         <v>5000000</v>
       </c>
       <c r="L131" s="113">
-        <f t="shared" ref="L131:N131" si="104">SUM(L132:L135)</f>
+        <f t="shared" ref="L131" si="104">SUM(L132:L135)</f>
         <v>5000000</v>
       </c>
       <c r="M131" s="113" cm="1">
@@ -15932,7 +15932,7 @@
         <v>48000000</v>
       </c>
       <c r="K136" s="125">
-        <f t="shared" ref="K136:N136" si="107">K137</f>
+        <f t="shared" ref="K136:L136" si="107">K137</f>
         <v>4000000</v>
       </c>
       <c r="L136" s="125">
@@ -16017,7 +16017,7 @@
         <v>2100000</v>
       </c>
       <c r="K138" s="119">
-        <f t="shared" ref="K138:N138" si="108">K139</f>
+        <f t="shared" ref="K138:L138" si="108">K139</f>
         <v>600000</v>
       </c>
       <c r="L138" s="119">
@@ -16158,7 +16158,7 @@
         <v>2500000</v>
       </c>
       <c r="L141" s="125">
-        <f t="shared" ref="L141:N141" si="112">SUM(L142:L143)</f>
+        <f t="shared" ref="L141" si="112">SUM(L142:L143)</f>
         <v>2500000</v>
       </c>
       <c r="M141" s="113" cm="1">
@@ -16278,7 +16278,7 @@
         <v>7800000</v>
       </c>
       <c r="K144" s="119">
-        <f t="shared" ref="K144:N144" si="115">K145</f>
+        <f t="shared" ref="K144:L144" si="115">K145</f>
         <v>0</v>
       </c>
       <c r="L144" s="119">
@@ -16363,7 +16363,7 @@
         <v>36540000</v>
       </c>
       <c r="L146" s="113">
-        <f t="shared" ref="L146:N146" si="117">SUM(L147:L148)</f>
+        <f t="shared" ref="L146" si="117">SUM(L147:L148)</f>
         <v>35540000</v>
       </c>
       <c r="M146" s="113" cm="1">
@@ -16539,7 +16539,7 @@
         <v>4500000</v>
       </c>
       <c r="L150" s="125">
-        <f t="shared" ref="L150:N150" si="123">SUM(L151:L154)</f>
+        <f t="shared" ref="L150" si="123">SUM(L151:L154)</f>
         <v>4500000</v>
       </c>
       <c r="M150" s="113" cm="1">
@@ -16737,7 +16737,7 @@
         <v>3000000</v>
       </c>
       <c r="K155" s="119">
-        <f t="shared" ref="K155:N155" si="126">K156</f>
+        <f t="shared" ref="K155:L155" si="126">K156</f>
         <v>0</v>
       </c>
       <c r="L155" s="119">
@@ -16818,7 +16818,7 @@
         <v>38000000</v>
       </c>
       <c r="K157" s="119">
-        <f t="shared" ref="K157:N157" si="127">K158</f>
+        <f t="shared" ref="K157:L157" si="127">K158</f>
         <v>4750000</v>
       </c>
       <c r="L157" s="119">
@@ -16903,7 +16903,7 @@
         <v>3000000</v>
       </c>
       <c r="K159" s="125">
-        <f t="shared" ref="K159:N159" si="128">K160</f>
+        <f t="shared" ref="K159:L159" si="128">K160</f>
         <v>300000</v>
       </c>
       <c r="L159" s="125">
@@ -17044,7 +17044,7 @@
         <v>5000000</v>
       </c>
       <c r="L162" s="119">
-        <f t="shared" ref="L162:N162" si="132">SUM(L163:L166)</f>
+        <f t="shared" ref="L162" si="132">SUM(L163:L166)</f>
         <v>5000000</v>
       </c>
       <c r="M162" s="113" cm="1">
@@ -17242,7 +17242,7 @@
         <v>40000000</v>
       </c>
       <c r="K167" s="119">
-        <f t="shared" ref="K167:N167" si="135">K168</f>
+        <f t="shared" ref="K167:L167" si="135">K168</f>
         <v>8000000</v>
       </c>
       <c r="L167" s="119">
@@ -17327,7 +17327,7 @@
         <v>3000000</v>
       </c>
       <c r="K169" s="119">
-        <f t="shared" ref="K169:N169" si="136">K170</f>
+        <f t="shared" ref="K169:L169" si="136">K170</f>
         <v>300000</v>
       </c>
       <c r="L169" s="119">
@@ -17468,7 +17468,7 @@
         <v>5000000</v>
       </c>
       <c r="L172" s="125">
-        <f t="shared" ref="L172:N172" si="140">SUM(L173:L176)</f>
+        <f t="shared" ref="L172" si="140">SUM(L173:L176)</f>
         <v>5000000</v>
       </c>
       <c r="M172" s="113" cm="1">
@@ -17666,7 +17666,7 @@
         <v>26250000</v>
       </c>
       <c r="K177" s="119">
-        <f t="shared" ref="K177:N177" si="143">K178</f>
+        <f t="shared" ref="K177:L177" si="143">K178</f>
         <v>3500000</v>
       </c>
       <c r="L177" s="119">
@@ -17751,7 +17751,7 @@
         <v>32435000</v>
       </c>
       <c r="K179" s="119">
-        <f t="shared" ref="K179:N179" si="144">K180</f>
+        <f t="shared" ref="K179:L179" si="144">K180</f>
         <v>8250000</v>
       </c>
       <c r="L179" s="119">
@@ -17836,7 +17836,7 @@
         <v>2100000</v>
       </c>
       <c r="K181" s="113">
-        <f t="shared" ref="K181:N181" si="145">K182</f>
+        <f t="shared" ref="K181:L181" si="145">K182</f>
         <v>300000</v>
       </c>
       <c r="L181" s="113">
@@ -17977,7 +17977,7 @@
         <v>0</v>
       </c>
       <c r="L184" s="119">
-        <f t="shared" ref="L184:N184" si="149">SUM(L185:L188)</f>
+        <f t="shared" ref="L184" si="149">SUM(L185:L188)</f>
         <v>0</v>
       </c>
       <c r="M184" s="113" cm="1">
@@ -18159,7 +18159,7 @@
         <v>3000000</v>
       </c>
       <c r="K189" s="119">
-        <f t="shared" ref="K189:N189" si="152">K190</f>
+        <f t="shared" ref="K189:L189" si="152">K190</f>
         <v>0</v>
       </c>
       <c r="L189" s="119">
@@ -18240,7 +18240,7 @@
         <v>9000000</v>
       </c>
       <c r="K191" s="119">
-        <f t="shared" ref="K191:N191" si="153">K192</f>
+        <f t="shared" ref="K191:L191" si="153">K192</f>
         <v>0</v>
       </c>
       <c r="L191" s="119">
@@ -18321,7 +18321,7 @@
         <v>18042000</v>
       </c>
       <c r="K193" s="119">
-        <f t="shared" ref="K193:N193" si="154">K194</f>
+        <f t="shared" ref="K193:L193" si="154">K194</f>
         <v>0</v>
       </c>
       <c r="L193" s="119">
@@ -18458,7 +18458,7 @@
         <v>3250000</v>
       </c>
       <c r="L196" s="113">
-        <f t="shared" ref="L196:N196" si="158">SUM(L197:L200)</f>
+        <f t="shared" ref="L196" si="158">SUM(L197:L200)</f>
         <v>3250000</v>
       </c>
       <c r="M196" s="113" cm="1">
@@ -18652,7 +18652,7 @@
         <v>3000000</v>
       </c>
       <c r="K201" s="119">
-        <f t="shared" ref="K201:N201" si="161">K202</f>
+        <f t="shared" ref="K201:L201" si="161">K202</f>
         <v>250000</v>
       </c>
       <c r="L201" s="119">
@@ -18737,7 +18737,7 @@
         <v>71534000</v>
       </c>
       <c r="K203" s="113">
-        <f t="shared" ref="K203:N203" si="162">K204</f>
+        <f t="shared" ref="K203:L203" si="162">K204</f>
         <v>15300000</v>
       </c>
       <c r="L203" s="113">
@@ -18878,7 +18878,7 @@
         <v>3250000</v>
       </c>
       <c r="L206" s="113">
-        <f t="shared" ref="L206:N206" si="166">SUM(L207:L210)</f>
+        <f t="shared" ref="L206" si="166">SUM(L207:L210)</f>
         <v>3250000</v>
       </c>
       <c r="M206" s="113" cm="1">
@@ -19072,7 +19072,7 @@
         <v>116054000</v>
       </c>
       <c r="K211" s="113">
-        <f t="shared" ref="K211:N211" si="169">K212</f>
+        <f t="shared" ref="K211:L211" si="169">K212</f>
         <v>0</v>
       </c>
       <c r="L211" s="113">
@@ -19209,7 +19209,7 @@
         <v>0</v>
       </c>
       <c r="L214" s="119">
-        <f t="shared" ref="L214:N214" si="173">SUM(L215:L218)</f>
+        <f t="shared" ref="L214" si="173">SUM(L215:L218)</f>
         <v>0</v>
       </c>
       <c r="M214" s="113" cm="1">
@@ -19391,7 +19391,7 @@
         <v>34500000</v>
       </c>
       <c r="K219" s="113">
-        <f t="shared" ref="K219:N219" si="176">K220</f>
+        <f t="shared" ref="K219:L219" si="176">K220</f>
         <v>0</v>
       </c>
       <c r="L219" s="113">
@@ -19622,7 +19622,7 @@
         <v>2230921700</v>
       </c>
       <c r="K224" s="125">
-        <f t="shared" ref="K224:N224" si="182">K225</f>
+        <f t="shared" ref="K224:L224" si="182">K225</f>
         <v>0</v>
       </c>
       <c r="L224" s="125">
@@ -19705,7 +19705,7 @@
         <v>106651</v>
       </c>
       <c r="K226" s="119">
-        <f t="shared" ref="K226:N226" si="183">K227</f>
+        <f t="shared" ref="K226:L226" si="183">K227</f>
         <v>0</v>
       </c>
       <c r="L226" s="119">
@@ -19788,7 +19788,7 @@
         <v>152433320</v>
       </c>
       <c r="K228" s="119">
-        <f t="shared" ref="K228:N228" si="184">K229</f>
+        <f t="shared" ref="K228:L228" si="184">K229</f>
         <v>0</v>
       </c>
       <c r="L228" s="119">
@@ -19871,7 +19871,7 @@
         <v>54170454</v>
       </c>
       <c r="K230" s="119">
-        <f t="shared" ref="K230:N230" si="185">K231</f>
+        <f t="shared" ref="K230:L230" si="185">K231</f>
         <v>0</v>
       </c>
       <c r="L230" s="119">
@@ -19954,7 +19954,7 @@
         <v>130450000</v>
       </c>
       <c r="K232" s="119">
-        <f t="shared" ref="K232:N232" si="186">K233</f>
+        <f t="shared" ref="K232:L232" si="186">K233</f>
         <v>0</v>
       </c>
       <c r="L232" s="119">
@@ -20037,7 +20037,7 @@
         <v>186546000</v>
       </c>
       <c r="K234" s="119">
-        <f t="shared" ref="K234:N234" si="187">K235</f>
+        <f t="shared" ref="K234:L234" si="187">K235</f>
         <v>0</v>
       </c>
       <c r="L234" s="119">
@@ -20120,7 +20120,7 @@
         <v>13039929</v>
       </c>
       <c r="K236" s="119">
-        <f t="shared" ref="K236:N236" si="188">K237</f>
+        <f t="shared" ref="K236:L236" si="188">K237</f>
         <v>0</v>
       </c>
       <c r="L236" s="119">
@@ -20203,7 +20203,7 @@
         <v>104945600</v>
       </c>
       <c r="K238" s="113">
-        <f t="shared" ref="K238:N238" si="189">K239</f>
+        <f t="shared" ref="K238:L238" si="189">K239</f>
         <v>0</v>
       </c>
       <c r="L238" s="113">
@@ -20286,7 +20286,7 @@
         <v>451220000</v>
       </c>
       <c r="K240" s="119">
-        <f t="shared" ref="K240:N240" si="190">K241</f>
+        <f t="shared" ref="K240:L240" si="190">K241</f>
         <v>0</v>
       </c>
       <c r="L240" s="119">
@@ -20367,7 +20367,7 @@
         <v>76680000</v>
       </c>
       <c r="K242" s="113">
-        <f t="shared" ref="K242:N242" si="191">K243</f>
+        <f t="shared" ref="K242:L242" si="191">K243</f>
         <v>0</v>
       </c>
       <c r="L242" s="113">
@@ -20450,7 +20450,7 @@
         <v>173032000</v>
       </c>
       <c r="K244" s="125">
-        <f t="shared" ref="K244:N244" si="192">K245</f>
+        <f t="shared" ref="K244:L244" si="192">K245</f>
         <v>0</v>
       </c>
       <c r="L244" s="125">
@@ -20531,7 +20531,7 @@
         <v>3257727000</v>
       </c>
       <c r="K246" s="119">
-        <f t="shared" ref="K246:N246" si="193">K247</f>
+        <f t="shared" ref="K246:L246" si="193">K247</f>
         <v>0</v>
       </c>
       <c r="L246" s="119">
@@ -20716,7 +20716,7 @@
         <v>0</v>
       </c>
       <c r="L250" s="119">
-        <f t="shared" ref="L250:N250" si="199">SUM(L251:L260)</f>
+        <f t="shared" ref="L250" si="199">SUM(L251:L260)</f>
         <v>0</v>
       </c>
       <c r="M250" s="113" cm="1">
@@ -21108,7 +21108,7 @@
         <v>103250000</v>
       </c>
       <c r="K261" s="113">
-        <f t="shared" ref="K261:N261" si="202">K262</f>
+        <f t="shared" ref="K261:L261" si="202">K262</f>
         <v>0</v>
       </c>
       <c r="L261" s="113">
@@ -21189,7 +21189,7 @@
         <v>0</v>
       </c>
       <c r="L263" s="164">
-        <f t="shared" ref="L263:N263" si="204">SUM(L264:L272)</f>
+        <f t="shared" ref="L263" si="204">SUM(L264:L272)</f>
         <v>0</v>
       </c>
       <c r="M263" s="113" cm="1">
@@ -21576,7 +21576,7 @@
         <v>30000000</v>
       </c>
       <c r="K274" s="119">
-        <f t="shared" ref="K274:N274" si="209">K275</f>
+        <f t="shared" ref="K274:L274" si="209">K275</f>
         <v>0</v>
       </c>
       <c r="L274" s="119">
@@ -21657,7 +21657,7 @@
         <v>0</v>
       </c>
       <c r="L276" s="113">
-        <f t="shared" ref="L276:N276" si="211">SUM(L277:L278)</f>
+        <f t="shared" ref="L276" si="211">SUM(L277:L278)</f>
         <v>0</v>
       </c>
       <c r="M276" s="113" cm="1">
@@ -21817,7 +21817,7 @@
         <v>0</v>
       </c>
       <c r="L280" s="119">
-        <f t="shared" ref="L280:N280" si="217">SUM(L281:L289)</f>
+        <f t="shared" ref="L280" si="217">SUM(L281:L289)</f>
         <v>0</v>
       </c>
       <c r="M280" s="113" cm="1">
@@ -22154,7 +22154,7 @@
         <v>36000000</v>
       </c>
       <c r="K290" s="119">
-        <f t="shared" ref="K290:N290" si="220">K291</f>
+        <f t="shared" ref="K290:L290" si="220">K291</f>
         <v>0</v>
       </c>
       <c r="L290" s="119">
@@ -22281,7 +22281,7 @@
         <v>79060000</v>
       </c>
       <c r="K293" s="113">
-        <f t="shared" ref="K293:N293" si="223">K294</f>
+        <f t="shared" ref="K293:L293" si="223">K294</f>
         <v>0</v>
       </c>
       <c r="L293" s="113">
@@ -22362,7 +22362,7 @@
         <v>0</v>
       </c>
       <c r="L295" s="119">
-        <f t="shared" ref="L295:N295" si="225">SUM(L296:L305)</f>
+        <f t="shared" ref="L295" si="225">SUM(L296:L305)</f>
         <v>0</v>
       </c>
       <c r="M295" s="113" cm="1">
@@ -23001,10 +23001,10 @@
       <c r="D312" s="280">
         <v>7</v>
       </c>
-      <c r="E312" s="297" t="s">
+      <c r="E312" s="299" t="s">
         <v>804</v>
       </c>
-      <c r="F312" s="298"/>
+      <c r="F312" s="300"/>
       <c r="G312" s="177">
         <f>SUM(G313,G384,G432)</f>
         <v>2633607000</v>
@@ -23221,7 +23221,7 @@
         <v>4000000</v>
       </c>
       <c r="L316" s="119">
-        <f t="shared" ref="L316:N316" si="238">SUM(L317:L321)</f>
+        <f t="shared" ref="L316" si="238">SUM(L317:L321)</f>
         <v>4000000</v>
       </c>
       <c r="M316" s="113" cm="1">
@@ -23450,7 +23450,7 @@
         <v>1000000</v>
       </c>
       <c r="K322" s="119">
-        <f t="shared" ref="K322:N322" si="241">K323</f>
+        <f t="shared" ref="K322:L322" si="241">K323</f>
         <v>0</v>
       </c>
       <c r="L322" s="119">
@@ -23531,7 +23531,7 @@
         <v>130000000</v>
       </c>
       <c r="K324" s="119">
-        <f t="shared" ref="K324:N324" si="242">K325</f>
+        <f t="shared" ref="K324:L324" si="242">K325</f>
         <v>0</v>
       </c>
       <c r="L324" s="119">
@@ -23668,7 +23668,7 @@
         <v>4000000</v>
       </c>
       <c r="L327" s="119">
-        <f t="shared" ref="L327:N327" si="246">SUM(L328:L332)</f>
+        <f t="shared" ref="L327" si="246">SUM(L328:L332)</f>
         <v>4000000</v>
       </c>
       <c r="M327" s="113" cm="1">
@@ -23897,7 +23897,7 @@
         <v>1000000</v>
       </c>
       <c r="K333" s="119">
-        <f t="shared" ref="K333:N333" si="249">K334</f>
+        <f t="shared" ref="K333:L333" si="249">K334</f>
         <v>0</v>
       </c>
       <c r="L333" s="119">
@@ -23978,7 +23978,7 @@
         <v>4000000</v>
       </c>
       <c r="K335" s="119">
-        <f t="shared" ref="K335:N335" si="250">K336</f>
+        <f t="shared" ref="K335:L335" si="250">K336</f>
         <v>0</v>
       </c>
       <c r="L335" s="119">
@@ -24059,7 +24059,7 @@
         <v>117000000</v>
       </c>
       <c r="K337" s="180">
-        <f t="shared" ref="K337:N337" si="251">K338</f>
+        <f t="shared" ref="K337:L337" si="251">K338</f>
         <v>0</v>
       </c>
       <c r="L337" s="180">
@@ -24196,7 +24196,7 @@
         <v>4000000</v>
       </c>
       <c r="L340" s="125">
-        <f t="shared" ref="L340:N340" si="255">SUM(L341:L345)</f>
+        <f t="shared" ref="L340" si="255">SUM(L341:L345)</f>
         <v>4000000</v>
       </c>
       <c r="M340" s="113" cm="1">
@@ -24425,7 +24425,7 @@
         <v>1000000</v>
       </c>
       <c r="K346" s="180">
-        <f t="shared" ref="K346:N346" si="258">K347</f>
+        <f t="shared" ref="K346:L346" si="258">K347</f>
         <v>0</v>
       </c>
       <c r="L346" s="180">
@@ -24506,7 +24506,7 @@
         <v>8000000</v>
       </c>
       <c r="K348" s="161">
-        <f t="shared" ref="K348:N348" si="259">K349</f>
+        <f t="shared" ref="K348:L348" si="259">K349</f>
         <v>0</v>
       </c>
       <c r="L348" s="161">
@@ -24587,7 +24587,7 @@
         <v>117435000</v>
       </c>
       <c r="K350" s="113">
-        <f t="shared" ref="K350:N350" si="260">K351</f>
+        <f t="shared" ref="K350:L350" si="260">K351</f>
         <v>0</v>
       </c>
       <c r="L350" s="113">
@@ -24724,7 +24724,7 @@
         <v>4000000</v>
       </c>
       <c r="L353" s="119">
-        <f t="shared" ref="L353:N353" si="264">SUM(L354:L357)</f>
+        <f t="shared" ref="L353" si="264">SUM(L354:L357)</f>
         <v>4000000</v>
       </c>
       <c r="M353" s="113" cm="1">
@@ -24918,7 +24918,7 @@
         <v>137500000</v>
       </c>
       <c r="K358" s="119">
-        <f t="shared" ref="K358:N358" si="267">K359</f>
+        <f t="shared" ref="K358:L358" si="267">K359</f>
         <v>0</v>
       </c>
       <c r="L358" s="119">
@@ -25055,7 +25055,7 @@
         <v>4000000</v>
       </c>
       <c r="L361" s="119">
-        <f t="shared" ref="L361:N361" si="271">SUM(L362:L365)</f>
+        <f t="shared" ref="L361" si="271">SUM(L362:L365)</f>
         <v>4000000</v>
       </c>
       <c r="M361" s="113" cm="1">
@@ -25249,7 +25249,7 @@
         <v>135937000</v>
       </c>
       <c r="K366" s="119">
-        <f t="shared" ref="K366:N366" si="274">K367</f>
+        <f t="shared" ref="K366:L366" si="274">K367</f>
         <v>0</v>
       </c>
       <c r="L366" s="119">
@@ -25386,7 +25386,7 @@
         <v>0</v>
       </c>
       <c r="L369" s="119">
-        <f t="shared" ref="L369:N369" si="278">SUM(L370:L375)</f>
+        <f t="shared" ref="L369" si="278">SUM(L370:L375)</f>
         <v>0</v>
       </c>
       <c r="M369" s="113" cm="1">
@@ -25638,7 +25638,7 @@
         <v>16000000</v>
       </c>
       <c r="K376" s="113">
-        <f t="shared" ref="K376:N376" si="281">K377</f>
+        <f t="shared" ref="K376:L376" si="281">K377</f>
         <v>0</v>
       </c>
       <c r="L376" s="113">
@@ -25719,7 +25719,7 @@
         <v>15000000</v>
       </c>
       <c r="K378" s="119">
-        <f t="shared" ref="K378:N378" si="282">K379</f>
+        <f t="shared" ref="K378:L378" si="282">K379</f>
         <v>0</v>
       </c>
       <c r="L378" s="119">
@@ -25804,7 +25804,7 @@
         <v>0</v>
       </c>
       <c r="L380" s="119">
-        <f t="shared" ref="L380:N380" si="284">SUM(L381:L383)</f>
+        <f t="shared" ref="L380" si="284">SUM(L381:L383)</f>
         <v>0</v>
       </c>
       <c r="M380" s="113" cm="1">
@@ -26105,7 +26105,7 @@
         <v>5000000</v>
       </c>
       <c r="L387" s="113">
-        <f t="shared" ref="L387:N387" si="294">SUM(L388:L392)</f>
+        <f t="shared" ref="L387" si="294">SUM(L388:L392)</f>
         <v>2375000</v>
       </c>
       <c r="M387" s="113" cm="1">
@@ -26342,7 +26342,7 @@
         <v>1000000</v>
       </c>
       <c r="K393" s="119">
-        <f t="shared" ref="K393:N393" si="297">K394</f>
+        <f t="shared" ref="K393:L393" si="297">K394</f>
         <v>250000</v>
       </c>
       <c r="L393" s="119">
@@ -26427,7 +26427,7 @@
         <v>109075000</v>
       </c>
       <c r="K395" s="119">
-        <f t="shared" ref="K395:N395" si="298">K396</f>
+        <f t="shared" ref="K395:L395" si="298">K396</f>
         <v>0</v>
       </c>
       <c r="L395" s="119">
@@ -26564,7 +26564,7 @@
         <v>1200000</v>
       </c>
       <c r="L398" s="119">
-        <f t="shared" ref="L398:N398" si="302">SUM(L399:L403)</f>
+        <f t="shared" ref="L398" si="302">SUM(L399:L403)</f>
         <v>600000</v>
       </c>
       <c r="M398" s="113" cm="1">
@@ -26789,7 +26789,7 @@
         <v>0</v>
       </c>
       <c r="L404" s="119">
-        <f t="shared" ref="L404:N404" si="306">SUM(L405:L406)</f>
+        <f t="shared" ref="L404" si="306">SUM(L405:L406)</f>
         <v>0</v>
       </c>
       <c r="M404" s="113" cm="1">
@@ -26901,7 +26901,7 @@
         <v>10000000</v>
       </c>
       <c r="K407" s="125">
-        <f t="shared" ref="K407:N407" si="309">K408</f>
+        <f t="shared" ref="K407:L407" si="309">K408</f>
         <v>0</v>
       </c>
       <c r="L407" s="125">
@@ -26982,7 +26982,7 @@
         <v>114306000</v>
       </c>
       <c r="K409" s="119">
-        <f t="shared" ref="K409:N409" si="310">K410</f>
+        <f t="shared" ref="K409:L409" si="310">K410</f>
         <v>0</v>
       </c>
       <c r="L409" s="119">
@@ -27119,7 +27119,7 @@
         <v>0</v>
       </c>
       <c r="L412" s="113">
-        <f t="shared" ref="L412:N412" si="314">SUM(L413:L417)</f>
+        <f t="shared" ref="L412" si="314">SUM(L413:L417)</f>
         <v>0</v>
       </c>
       <c r="M412" s="113" cm="1">
@@ -27336,7 +27336,7 @@
         <v>1000000</v>
       </c>
       <c r="K418" s="113">
-        <f t="shared" ref="K418:N418" si="317">K419</f>
+        <f t="shared" ref="K418:L418" si="317">K419</f>
         <v>0</v>
       </c>
       <c r="L418" s="113">
@@ -27417,7 +27417,7 @@
         <v>283540000</v>
       </c>
       <c r="K420" s="113">
-        <f t="shared" ref="K420:N420" si="318">K421</f>
+        <f t="shared" ref="K420:L420" si="318">K421</f>
         <v>0</v>
       </c>
       <c r="L420" s="113">
@@ -27602,7 +27602,7 @@
         <v>7100000</v>
       </c>
       <c r="L424" s="119">
-        <f t="shared" ref="L424:N424" si="323">SUM(L425:L429)</f>
+        <f t="shared" ref="L424" si="323">SUM(L425:L429)</f>
         <v>2250000</v>
       </c>
       <c r="M424" s="113" cm="1">
@@ -27839,7 +27839,7 @@
         <v>68811000</v>
       </c>
       <c r="K430" s="119">
-        <f t="shared" ref="K430:N430" si="326">K431</f>
+        <f t="shared" ref="K430:L430" si="326">K431</f>
         <v>4580000</v>
       </c>
       <c r="L430" s="119">
@@ -28079,7 +28079,7 @@
         <v>4000000</v>
       </c>
       <c r="L435" s="125">
-        <f t="shared" ref="L435:N435" si="333">SUM(L436:L439)</f>
+        <f t="shared" ref="L435" si="333">SUM(L436:L439)</f>
         <v>4000000</v>
       </c>
       <c r="M435" s="113" cm="1">
@@ -28273,7 +28273,7 @@
         <v>37528000</v>
       </c>
       <c r="K440" s="119">
-        <f t="shared" ref="K440:N440" si="336">K441</f>
+        <f t="shared" ref="K440:L440" si="336">K441</f>
         <v>0</v>
       </c>
       <c r="L440" s="119">
@@ -28354,7 +28354,7 @@
         <v>3600000</v>
       </c>
       <c r="K442" s="113">
-        <f t="shared" ref="K442:N442" si="337">K443</f>
+        <f t="shared" ref="K442:L442" si="337">K443</f>
         <v>0</v>
       </c>
       <c r="L442" s="113">
@@ -28491,7 +28491,7 @@
         <v>1500000</v>
       </c>
       <c r="L445" s="125">
-        <f t="shared" ref="L445:N445" si="341">SUM(L446:L449)</f>
+        <f t="shared" ref="L445" si="341">SUM(L446:L449)</f>
         <v>1500000</v>
       </c>
       <c r="M445" s="113" cm="1">
@@ -28677,7 +28677,7 @@
         <v>32120000</v>
       </c>
       <c r="K450" s="113">
-        <f t="shared" ref="K450:N450" si="344">K451</f>
+        <f t="shared" ref="K450:L450" si="344">K451</f>
         <v>5200000</v>
       </c>
       <c r="L450" s="113">
@@ -28763,7 +28763,7 @@
         <v>1200000</v>
       </c>
       <c r="K452" s="125">
-        <f t="shared" ref="K452:N452" si="345">K453</f>
+        <f t="shared" ref="K452:L452" si="345">K453</f>
         <v>0</v>
       </c>
       <c r="L452" s="125">
@@ -28900,7 +28900,7 @@
         <v>4660000</v>
       </c>
       <c r="L455" s="119">
-        <f t="shared" ref="L455:N455" si="349">SUM(L456:L460)</f>
+        <f t="shared" ref="L455" si="349">SUM(L456:L460)</f>
         <v>2660000</v>
       </c>
       <c r="M455" s="113" cm="1">
@@ -29133,7 +29133,7 @@
         <v>40320000</v>
       </c>
       <c r="K461" s="119">
-        <f t="shared" ref="K461:N461" si="352">K462</f>
+        <f t="shared" ref="K461:L461" si="352">K462</f>
         <v>5200000</v>
       </c>
       <c r="L461" s="119">
@@ -29219,7 +29219,7 @@
         <v>1800000</v>
       </c>
       <c r="K463" s="119">
-        <f t="shared" ref="K463:N463" si="353">K464</f>
+        <f t="shared" ref="K463:L463" si="353">K464</f>
         <v>0</v>
       </c>
       <c r="L463" s="119">
@@ -29356,7 +29356,7 @@
         <v>0</v>
       </c>
       <c r="L466" s="119">
-        <f t="shared" ref="L466:N466" si="357">SUM(L467:L470)</f>
+        <f t="shared" ref="L466" si="357">SUM(L467:L470)</f>
         <v>0</v>
       </c>
       <c r="M466" s="113" cm="1">
@@ -29538,7 +29538,7 @@
         <v>21379000</v>
       </c>
       <c r="K471" s="125">
-        <f t="shared" ref="K471:N471" si="360">K472</f>
+        <f t="shared" ref="K471:L471" si="360">K472</f>
         <v>11200000</v>
       </c>
       <c r="L471" s="125">
@@ -29623,7 +29623,7 @@
         <v>1500000</v>
       </c>
       <c r="K473" s="119">
-        <f t="shared" ref="K473:N473" si="361">K474</f>
+        <f t="shared" ref="K473:L473" si="361">K474</f>
         <v>0</v>
       </c>
       <c r="L473" s="119">
@@ -29760,7 +29760,7 @@
         <v>660000</v>
       </c>
       <c r="L476" s="119">
-        <f t="shared" ref="L476:N476" si="365">SUM(L477:L480)</f>
+        <f t="shared" ref="L476" si="365">SUM(L477:L480)</f>
         <v>660000</v>
       </c>
       <c r="M476" s="113" cm="1">
@@ -29946,7 +29946,7 @@
         <v>35003000</v>
       </c>
       <c r="K481" s="113">
-        <f t="shared" ref="K481:N481" si="368">K482</f>
+        <f t="shared" ref="K481:L481" si="368">K482</f>
         <v>5200000</v>
       </c>
       <c r="L481" s="113">
@@ -30031,7 +30031,7 @@
         <v>1800000</v>
       </c>
       <c r="K483" s="119">
-        <f t="shared" ref="K483:N483" si="369">K484</f>
+        <f t="shared" ref="K483:L483" si="369">K484</f>
         <v>0</v>
       </c>
       <c r="L483" s="119">
@@ -30168,7 +30168,7 @@
         <v>0</v>
       </c>
       <c r="L486" s="113">
-        <f t="shared" ref="L486:N486" si="373">SUM(L487:L490)</f>
+        <f t="shared" ref="L486" si="373">SUM(L487:L490)</f>
         <v>0</v>
       </c>
       <c r="M486" s="113" cm="1">
@@ -30350,7 +30350,7 @@
         <v>10000000</v>
       </c>
       <c r="K491" s="125">
-        <f t="shared" ref="K491:N491" si="376">K492</f>
+        <f t="shared" ref="K491:L491" si="376">K492</f>
         <v>0</v>
       </c>
       <c r="L491" s="125">
@@ -30431,7 +30431,7 @@
         <v>127000000</v>
       </c>
       <c r="K493" s="119">
-        <f t="shared" ref="K493:N493" si="377">K494</f>
+        <f t="shared" ref="K493:L493" si="377">K494</f>
         <v>0</v>
       </c>
       <c r="L493" s="119">
@@ -30568,7 +30568,7 @@
         <v>0</v>
       </c>
       <c r="L496" s="119">
-        <f t="shared" ref="L496:N496" si="381">SUM(L497:L500)</f>
+        <f t="shared" ref="L496" si="381">SUM(L497:L500)</f>
         <v>0</v>
       </c>
       <c r="M496" s="113" cm="1">
@@ -30750,7 +30750,7 @@
         <v>20000000</v>
       </c>
       <c r="K501" s="119">
-        <f t="shared" ref="K501:N501" si="384">K502</f>
+        <f t="shared" ref="K501:L501" si="384">K502</f>
         <v>0</v>
       </c>
       <c r="L501" s="119">
@@ -30831,7 +30831,7 @@
         <v>43303000</v>
       </c>
       <c r="K503" s="119">
-        <f t="shared" ref="K503:N503" si="385">K504</f>
+        <f t="shared" ref="K503:L503" si="385">K504</f>
         <v>0</v>
       </c>
       <c r="L503" s="119">
@@ -30942,10 +30942,10 @@
       <c r="D506" s="175">
         <v>235</v>
       </c>
-      <c r="E506" s="297" t="s">
+      <c r="E506" s="299" t="s">
         <v>945</v>
       </c>
-      <c r="F506" s="299"/>
+      <c r="F506" s="301"/>
       <c r="G506" s="177">
         <f>G507</f>
         <v>8500000000</v>
@@ -31162,7 +31162,7 @@
         <v>0</v>
       </c>
       <c r="L510" s="113">
-        <f t="shared" ref="L510:N510" si="394">SUM(L511:L516)</f>
+        <f t="shared" ref="L510" si="394">SUM(L511:L516)</f>
         <v>0</v>
       </c>
       <c r="M510" s="113" cm="1">
@@ -31418,7 +31418,7 @@
         <v>0</v>
       </c>
       <c r="L517" s="119">
-        <f t="shared" ref="L517:N517" si="398">SUM(L518:L519)</f>
+        <f t="shared" ref="L517" si="398">SUM(L518:L519)</f>
         <v>0</v>
       </c>
       <c r="M517" s="113" cm="1">
@@ -31530,7 +31530,7 @@
         <v>10000000</v>
       </c>
       <c r="K520" s="119">
-        <f t="shared" ref="K520:N520" si="401">K521</f>
+        <f t="shared" ref="K520:L520" si="401">K521</f>
         <v>0</v>
       </c>
       <c r="L520" s="119">
@@ -31611,7 +31611,7 @@
         <v>76950000</v>
       </c>
       <c r="K522" s="119">
-        <f t="shared" ref="K522:N522" si="402">K523</f>
+        <f t="shared" ref="K522:L522" si="402">K523</f>
         <v>0</v>
       </c>
       <c r="L522" s="119">
@@ -31696,7 +31696,7 @@
         <v>0</v>
       </c>
       <c r="L524" s="125">
-        <f t="shared" ref="L524:N524" si="404">SUM(L525:L526)</f>
+        <f t="shared" ref="L524" si="404">SUM(L525:L526)</f>
         <v>0</v>
       </c>
       <c r="M524" s="113" cm="1">
@@ -31864,7 +31864,7 @@
         <v>0</v>
       </c>
       <c r="L528" s="113">
-        <f t="shared" ref="L528:N528" si="410">SUM(L529:L534)</f>
+        <f t="shared" ref="L528" si="410">SUM(L529:L534)</f>
         <v>0</v>
       </c>
       <c r="M528" s="113" cm="1">
@@ -32120,7 +32120,7 @@
         <v>0</v>
       </c>
       <c r="L535" s="119">
-        <f t="shared" ref="L535:N535" si="414">SUM(L536:L537)</f>
+        <f t="shared" ref="L535" si="414">SUM(L536:L537)</f>
         <v>0</v>
       </c>
       <c r="M535" s="113" cm="1">
@@ -32232,7 +32232,7 @@
         <v>20000000</v>
       </c>
       <c r="K538" s="119">
-        <f t="shared" ref="K538:N538" si="417">K539</f>
+        <f t="shared" ref="K538:L538" si="417">K539</f>
         <v>0</v>
       </c>
       <c r="L538" s="119">
@@ -32317,7 +32317,7 @@
         <v>0</v>
       </c>
       <c r="L540" s="119">
-        <f t="shared" ref="L540:N540" si="419">SUM(L541:L542)</f>
+        <f t="shared" ref="L540" si="419">SUM(L541:L542)</f>
         <v>0</v>
       </c>
       <c r="M540" s="113" cm="1">
@@ -32433,7 +32433,7 @@
         <v>0</v>
       </c>
       <c r="L543" s="119">
-        <f t="shared" ref="L543:N543" si="423">SUM(L544:L546)</f>
+        <f t="shared" ref="L543" si="423">SUM(L544:L546)</f>
         <v>0</v>
       </c>
       <c r="M543" s="113" cm="1">
@@ -32636,7 +32636,7 @@
         <v>0</v>
       </c>
       <c r="L548" s="119">
-        <f t="shared" ref="L548:N548" si="429">SUM(L549:L551)</f>
+        <f t="shared" ref="L548" si="429">SUM(L549:L551)</f>
         <v>0</v>
       </c>
       <c r="M548" s="113" cm="1">
@@ -32783,7 +32783,7 @@
         <v>20000000</v>
       </c>
       <c r="K552" s="119">
-        <f t="shared" ref="K552:N552" si="432">K553</f>
+        <f t="shared" ref="K552:L552" si="432">K553</f>
         <v>0</v>
       </c>
       <c r="L552" s="119">
@@ -32864,7 +32864,7 @@
         <v>142041000</v>
       </c>
       <c r="K554" s="119">
-        <f t="shared" ref="K554:N554" si="433">K555</f>
+        <f t="shared" ref="K554:L554" si="433">K555</f>
         <v>0</v>
       </c>
       <c r="L554" s="119">
@@ -33049,7 +33049,7 @@
         <v>0</v>
       </c>
       <c r="L558" s="119">
-        <f t="shared" ref="L558:N558" si="438">SUM(L559:L562)</f>
+        <f t="shared" ref="L558" si="438">SUM(L559:L562)</f>
         <v>0</v>
       </c>
       <c r="M558" s="113" cm="1">
@@ -33231,7 +33231,7 @@
         <v>52170000</v>
       </c>
       <c r="K563" s="119">
-        <f t="shared" ref="K563:N563" si="441">K564</f>
+        <f t="shared" ref="K563:L563" si="441">K564</f>
         <v>0</v>
       </c>
       <c r="L563" s="119">
@@ -33297,7 +33297,7 @@
       <c r="D566" s="7"/>
       <c r="F566" s="8"/>
       <c r="G566" s="66" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="I566" s="2"/>
     </row>
@@ -33315,7 +33315,7 @@
       <c r="D568" s="7"/>
       <c r="F568" s="8"/>
       <c r="G568" s="66" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="I568" s="2"/>
     </row>
@@ -33343,7 +33343,7 @@
       </c>
       <c r="I571" s="2"/>
       <c r="J571" s="199" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="572" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -33356,7 +33356,7 @@
       </c>
       <c r="I572" s="2"/>
       <c r="J572" s="199" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="573" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -36961,7 +36961,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.35433070866141736" top="0.6692913385826772" bottom="1.0236220472440944" header="0" footer="0.39370078740157483"/>
-  <pageSetup paperSize="9" scale="56" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="57" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;LUsulan TUP 1 Pusdik KP, TA. 2023&amp;RHal &amp;P dari &amp;N</oddFooter>
   </headerFooter>
@@ -36982,7 +36982,7 @@
   <dimension ref="B2:XEW997"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -37002,17 +37002,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16377" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="313" t="s">
-        <v>986</v>
-      </c>
-      <c r="C2" s="313"/>
-      <c r="D2" s="313"/>
-      <c r="E2" s="313"/>
-      <c r="F2" s="313"/>
-      <c r="G2" s="313"/>
-      <c r="H2" s="313"/>
-      <c r="I2" s="313"/>
-      <c r="J2" s="313"/>
+      <c r="B2" s="307" t="s">
+        <v>985</v>
+      </c>
+      <c r="C2" s="307"/>
+      <c r="D2" s="307"/>
+      <c r="E2" s="307"/>
+      <c r="F2" s="307"/>
+      <c r="G2" s="307"/>
+      <c r="H2" s="307"/>
+      <c r="I2" s="307"/>
+      <c r="J2" s="307"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
@@ -53382,17 +53382,17 @@
       <c r="XEW2" s="3"/>
     </row>
     <row r="3" spans="2:16377" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="314" t="s">
+      <c r="B3" s="308" t="s">
         <v>521</v>
       </c>
-      <c r="C3" s="314"/>
-      <c r="D3" s="314"/>
-      <c r="E3" s="314"/>
-      <c r="F3" s="314"/>
-      <c r="G3" s="314"/>
-      <c r="H3" s="314"/>
-      <c r="I3" s="314"/>
-      <c r="J3" s="314"/>
+      <c r="C3" s="308"/>
+      <c r="D3" s="308"/>
+      <c r="E3" s="308"/>
+      <c r="F3" s="308"/>
+      <c r="G3" s="308"/>
+      <c r="H3" s="308"/>
+      <c r="I3" s="308"/>
+      <c r="J3" s="308"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -69763,42 +69763,42 @@
     </row>
     <row r="4" spans="2:16377" x14ac:dyDescent="0.25"/>
     <row r="5" spans="2:16377" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="315" t="s">
+      <c r="B5" s="309" t="s">
         <v>522</v>
       </c>
-      <c r="C5" s="316"/>
+      <c r="C5" s="310"/>
       <c r="D5" s="20" t="s">
         <v>523</v>
       </c>
     </row>
     <row r="6" spans="2:16377" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="317" t="s">
+      <c r="B6" s="311" t="s">
         <v>524</v>
       </c>
-      <c r="C6" s="318" t="s">
+      <c r="C6" s="312" t="s">
         <v>525</v>
       </c>
-      <c r="D6" s="318" t="s">
+      <c r="D6" s="312" t="s">
         <v>526</v>
       </c>
-      <c r="E6" s="319" t="str">
+      <c r="E6" s="314" t="str">
         <f>"Pagu "</f>
         <v xml:space="preserve">Pagu </v>
       </c>
-      <c r="F6" s="320" t="s">
+      <c r="F6" s="316" t="s">
         <v>520</v>
       </c>
-      <c r="G6" s="322" t="s">
+      <c r="G6" s="318" t="s">
         <v>969</v>
       </c>
-      <c r="H6" s="324" t="s">
-        <v>987</v>
-      </c>
-      <c r="I6" s="326" t="s">
+      <c r="H6" s="320" t="s">
+        <v>986</v>
+      </c>
+      <c r="I6" s="322" t="s">
+        <v>989</v>
+      </c>
+      <c r="J6" s="324" t="s">
         <v>970</v>
-      </c>
-      <c r="J6" s="328" t="s">
-        <v>971</v>
       </c>
       <c r="K6" s="21"/>
       <c r="L6" s="21"/>
@@ -69807,15 +69807,15 @@
       <c r="O6" s="21"/>
     </row>
     <row r="7" spans="2:16377" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="308"/>
-      <c r="C7" s="305"/>
-      <c r="D7" s="305"/>
-      <c r="E7" s="304"/>
-      <c r="F7" s="321"/>
-      <c r="G7" s="323"/>
-      <c r="H7" s="325"/>
-      <c r="I7" s="327"/>
-      <c r="J7" s="329"/>
+      <c r="B7" s="306"/>
+      <c r="C7" s="313"/>
+      <c r="D7" s="313"/>
+      <c r="E7" s="315"/>
+      <c r="F7" s="317"/>
+      <c r="G7" s="319"/>
+      <c r="H7" s="321"/>
+      <c r="I7" s="323"/>
+      <c r="J7" s="325"/>
       <c r="K7" s="21"/>
       <c r="L7" s="21"/>
       <c r="M7" s="21"/>
@@ -69826,10 +69826,10 @@
       <c r="B8" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="310" t="s">
+      <c r="C8" s="302" t="s">
         <v>527</v>
       </c>
-      <c r="D8" s="311"/>
+      <c r="D8" s="303"/>
       <c r="E8" s="23"/>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -69843,10 +69843,10 @@
       <c r="O8" s="25"/>
     </row>
     <row r="9" spans="2:16377" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="312">
+      <c r="B9" s="304">
         <v>1</v>
       </c>
-      <c r="C9" s="303" t="s">
+      <c r="C9" s="329" t="s">
         <v>500</v>
       </c>
       <c r="D9" s="26" t="s">
@@ -69865,13 +69865,16 @@
         <v>48600000</v>
       </c>
       <c r="H9" s="28" cm="1">
-        <f t="array" ref="H9">SUM(_xlfn._xlws.FILTER('Usulan TUP 1'!$L$15:$L$564,'Usulan TUP 1'!$P$15:$P$564=D9,0))</f>
+        <f t="array" ref="H9">SUM(_xlfn._xlws.FILTER('Usulan TUP 1'!$L$15:$L$564,'Usulan TUP 1'!$P$15:$P$564=$D9,0))</f>
         <v>40860000</v>
       </c>
-      <c r="I9" s="29"/>
+      <c r="I9" s="29" cm="1">
+        <f t="array" ref="I9">SUM(_xlfn._xlws.FILTER('Usulan TUP 1'!$M$15:$M$564,'Usulan TUP 1'!$P$15:$P$564=$D9,0))</f>
+        <v>20805701</v>
+      </c>
       <c r="J9" s="30">
         <f>H9-I9</f>
-        <v>40860000</v>
+        <v>20054299</v>
       </c>
       <c r="K9" s="31"/>
       <c r="L9" s="31"/>
@@ -69880,8 +69883,8 @@
       <c r="O9" s="31"/>
     </row>
     <row r="10" spans="2:16377" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="307"/>
-      <c r="C10" s="304"/>
+      <c r="B10" s="305"/>
+      <c r="C10" s="315"/>
       <c r="D10" s="32" t="s">
         <v>502</v>
       </c>
@@ -69898,13 +69901,16 @@
         <v>33540000</v>
       </c>
       <c r="H10" s="28" cm="1">
-        <f t="array" ref="H10">SUM(_xlfn._xlws.FILTER('Usulan TUP 1'!$L$15:$L$564,'Usulan TUP 1'!$P$15:$P$564=D10,0))</f>
+        <f t="array" ref="H10">SUM(_xlfn._xlws.FILTER('Usulan TUP 1'!$L$15:$L$564,'Usulan TUP 1'!$P$15:$P$564=$D10,0))</f>
         <v>24020000</v>
       </c>
-      <c r="I10" s="29"/>
+      <c r="I10" s="29" cm="1">
+        <f t="array" ref="I10">SUM(_xlfn._xlws.FILTER('Usulan TUP 1'!$M$15:$M$564,'Usulan TUP 1'!$P$15:$P$564=$D10,0))</f>
+        <v>13463000</v>
+      </c>
       <c r="J10" s="30">
         <f>H10-I10</f>
-        <v>24020000</v>
+        <v>10557000</v>
       </c>
       <c r="K10" s="31"/>
       <c r="L10" s="31"/>
@@ -69913,8 +69919,8 @@
       <c r="O10" s="31"/>
     </row>
     <row r="11" spans="2:16377" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="308"/>
-      <c r="C11" s="305"/>
+      <c r="B11" s="306"/>
+      <c r="C11" s="313"/>
       <c r="D11" s="60" t="s">
         <v>528</v>
       </c>
@@ -69935,12 +69941,12 @@
         <v>64880000</v>
       </c>
       <c r="I11" s="62">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="I11" si="1">SUM(I9:I10)</f>
+        <v>34268701</v>
       </c>
       <c r="J11" s="62">
         <f t="shared" si="0"/>
-        <v>64880000</v>
+        <v>30611299</v>
       </c>
       <c r="K11" s="81"/>
       <c r="L11" s="31"/>
@@ -69949,10 +69955,10 @@
       <c r="O11" s="31"/>
     </row>
     <row r="12" spans="2:16377" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="306">
+      <c r="B12" s="330">
         <v>2</v>
       </c>
-      <c r="C12" s="303" t="s">
+      <c r="C12" s="329" t="s">
         <v>508</v>
       </c>
       <c r="D12" s="33" t="s">
@@ -69971,13 +69977,16 @@
         <v>24000000</v>
       </c>
       <c r="H12" s="196" cm="1">
-        <f t="array" ref="H12">SUM(_xlfn._xlws.FILTER('Usulan TUP 1'!$L$15:$L$564,'Usulan TUP 1'!$P$15:$P$564=D12,0))</f>
+        <f t="array" ref="H12">SUM(_xlfn._xlws.FILTER('Usulan TUP 1'!$L$15:$L$564,'Usulan TUP 1'!$P$15:$P$564=$D12,0))</f>
         <v>24000000</v>
       </c>
-      <c r="I12" s="29"/>
+      <c r="I12" s="29" cm="1">
+        <f t="array" ref="I12">SUM(_xlfn._xlws.FILTER('Usulan TUP 1'!$M$15:$M$564,'Usulan TUP 1'!$P$15:$P$564=$D12,0))</f>
+        <v>23084500</v>
+      </c>
       <c r="J12" s="30">
         <f>H12-I12</f>
-        <v>24000000</v>
+        <v>915500</v>
       </c>
       <c r="K12" s="81"/>
       <c r="L12" s="81"/>
@@ -69986,8 +69995,8 @@
       <c r="O12" s="31"/>
     </row>
     <row r="13" spans="2:16377" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="307"/>
-      <c r="C13" s="304"/>
+      <c r="B13" s="305"/>
+      <c r="C13" s="315"/>
       <c r="D13" s="33" t="s">
         <v>510</v>
       </c>
@@ -70004,16 +70013,16 @@
         <v>18130000</v>
       </c>
       <c r="H13" s="28" cm="1">
-        <f t="array" ref="H13">SUM(_xlfn._xlws.FILTER('Usulan TUP 1'!$L$15:$L$564,'Usulan TUP 1'!$P$15:$P$564=D13,0))</f>
+        <f t="array" ref="H13">SUM(_xlfn._xlws.FILTER('Usulan TUP 1'!$L$15:$L$564,'Usulan TUP 1'!$P$15:$P$564=$D13,0))</f>
         <v>9065000</v>
       </c>
-      <c r="I13" s="29">
-        <f>H13</f>
-        <v>9065000</v>
+      <c r="I13" s="29" cm="1">
+        <f t="array" ref="I13">SUM(_xlfn._xlws.FILTER('Usulan TUP 1'!$M$15:$M$564,'Usulan TUP 1'!$P$15:$P$564=$D13,0))</f>
+        <v>9063948</v>
       </c>
       <c r="J13" s="30">
         <f>H13-I13</f>
-        <v>0</v>
+        <v>1052</v>
       </c>
       <c r="K13" s="31"/>
       <c r="L13" s="31"/>
@@ -70022,34 +70031,34 @@
       <c r="O13" s="31"/>
     </row>
     <row r="14" spans="2:16377" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="308"/>
-      <c r="C14" s="305"/>
+      <c r="B14" s="306"/>
+      <c r="C14" s="313"/>
       <c r="D14" s="60" t="s">
         <v>529</v>
       </c>
       <c r="E14" s="61">
-        <f t="shared" ref="E14:J14" si="1">SUM(E12:E13)</f>
+        <f t="shared" ref="E14:J14" si="2">SUM(E12:E13)</f>
         <v>10908584000</v>
       </c>
       <c r="F14" s="61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10908584000</v>
       </c>
       <c r="G14" s="62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>42130000</v>
       </c>
       <c r="H14" s="62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>33065000</v>
       </c>
       <c r="I14" s="62">
-        <f t="shared" si="1"/>
-        <v>9065000</v>
+        <f t="shared" ref="I14" si="3">SUM(I12:I13)</f>
+        <v>32148448</v>
       </c>
       <c r="J14" s="62">
-        <f t="shared" si="1"/>
-        <v>24000000</v>
+        <f t="shared" si="2"/>
+        <v>916552</v>
       </c>
       <c r="K14" s="81"/>
       <c r="L14" s="31"/>
@@ -70058,10 +70067,10 @@
       <c r="O14" s="31"/>
     </row>
     <row r="15" spans="2:16377" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="306">
+      <c r="B15" s="330">
         <v>3</v>
       </c>
-      <c r="C15" s="303" t="s">
+      <c r="C15" s="329" t="s">
         <v>503</v>
       </c>
       <c r="D15" s="33" t="s">
@@ -70080,13 +70089,16 @@
         <v>42500000</v>
       </c>
       <c r="H15" s="28" cm="1">
-        <f t="array" ref="H15">SUM(_xlfn._xlws.FILTER('Usulan TUP 1'!$L$15:$L$564,'Usulan TUP 1'!$P$15:$P$564=D15,0))</f>
+        <f t="array" ref="H15">SUM(_xlfn._xlws.FILTER('Usulan TUP 1'!$L$15:$L$564,'Usulan TUP 1'!$P$15:$P$564=$D15,0))</f>
         <v>30430000</v>
       </c>
-      <c r="I15" s="29"/>
+      <c r="I15" s="29" cm="1">
+        <f t="array" ref="I15">SUM(_xlfn._xlws.FILTER('Usulan TUP 1'!$M$15:$M$564,'Usulan TUP 1'!$P$15:$P$564=$D15,0))</f>
+        <v>29305120</v>
+      </c>
       <c r="J15" s="30">
         <f>H15-I15</f>
-        <v>30430000</v>
+        <v>1124880</v>
       </c>
       <c r="K15" s="31"/>
       <c r="L15" s="83"/>
@@ -70095,8 +70107,8 @@
       <c r="O15" s="31"/>
     </row>
     <row r="16" spans="2:16377" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="307"/>
-      <c r="C16" s="304"/>
+      <c r="B16" s="305"/>
+      <c r="C16" s="315"/>
       <c r="D16" s="33" t="s">
         <v>505</v>
       </c>
@@ -70113,13 +70125,16 @@
         <v>41300000</v>
       </c>
       <c r="H16" s="28" cm="1">
-        <f t="array" ref="H16">SUM(_xlfn._xlws.FILTER('Usulan TUP 1'!$L$15:$L$564,'Usulan TUP 1'!$P$15:$P$564=D16,0))</f>
+        <f t="array" ref="H16">SUM(_xlfn._xlws.FILTER('Usulan TUP 1'!$L$15:$L$564,'Usulan TUP 1'!$P$15:$P$564=$D16,0))</f>
         <v>27650000</v>
       </c>
-      <c r="I16" s="29"/>
+      <c r="I16" s="29" cm="1">
+        <f t="array" ref="I16">SUM(_xlfn._xlws.FILTER('Usulan TUP 1'!$M$15:$M$564,'Usulan TUP 1'!$P$15:$P$564=$D16,0))</f>
+        <v>26862500</v>
+      </c>
       <c r="J16" s="30">
         <f>H16-I16</f>
-        <v>27650000</v>
+        <v>787500</v>
       </c>
       <c r="K16" s="31"/>
       <c r="L16" s="31"/>
@@ -70128,34 +70143,34 @@
       <c r="O16" s="31"/>
     </row>
     <row r="17" spans="2:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="308"/>
-      <c r="C17" s="305"/>
+      <c r="B17" s="306"/>
+      <c r="C17" s="313"/>
       <c r="D17" s="60" t="s">
         <v>530</v>
       </c>
       <c r="E17" s="61">
-        <f t="shared" ref="E17:J17" si="2">SUM(E15:E16)</f>
+        <f t="shared" ref="E17:J17" si="4">SUM(E15:E16)</f>
         <v>745048000</v>
       </c>
       <c r="F17" s="61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>745048000</v>
       </c>
       <c r="G17" s="62">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>83800000</v>
       </c>
       <c r="H17" s="62">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>58080000</v>
       </c>
       <c r="I17" s="62">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" ref="I17" si="5">SUM(I15:I16)</f>
+        <v>56167620</v>
       </c>
       <c r="J17" s="62">
-        <f t="shared" si="2"/>
-        <v>58080000</v>
+        <f t="shared" si="4"/>
+        <v>1912380</v>
       </c>
       <c r="K17" s="81"/>
       <c r="L17" s="81"/>
@@ -70164,10 +70179,10 @@
       <c r="O17" s="31"/>
     </row>
     <row r="18" spans="2:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="306">
+      <c r="B18" s="330">
         <v>4</v>
       </c>
-      <c r="C18" s="303" t="s">
+      <c r="C18" s="329" t="s">
         <v>506</v>
       </c>
       <c r="D18" s="33" t="s">
@@ -70186,16 +70201,16 @@
         <v>88540000</v>
       </c>
       <c r="H18" s="28" cm="1">
-        <f t="array" ref="H18">SUM(_xlfn._xlws.FILTER('Usulan TUP 1'!$L$15:$L$564,'Usulan TUP 1'!$P$15:$P$564=D18,0))</f>
+        <f t="array" ref="H18">SUM(_xlfn._xlws.FILTER('Usulan TUP 1'!$L$15:$L$564,'Usulan TUP 1'!$P$15:$P$564=$D18,0))</f>
         <v>84540000</v>
       </c>
-      <c r="I18" s="29">
-        <f t="shared" ref="I18:I19" si="3">H18</f>
-        <v>84540000</v>
+      <c r="I18" s="29" cm="1">
+        <f t="array" ref="I18">SUM(_xlfn._xlws.FILTER('Usulan TUP 1'!$M$15:$M$564,'Usulan TUP 1'!$P$15:$P$564=$D18,0))</f>
+        <v>59045795</v>
       </c>
       <c r="J18" s="30">
         <f>H18-I18</f>
-        <v>0</v>
+        <v>25494205</v>
       </c>
       <c r="K18" s="31"/>
       <c r="L18" s="31"/>
@@ -70204,8 +70219,8 @@
       <c r="O18" s="31"/>
     </row>
     <row r="19" spans="2:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="307"/>
-      <c r="C19" s="304"/>
+      <c r="B19" s="305"/>
+      <c r="C19" s="315"/>
       <c r="D19" s="78" t="s">
         <v>511</v>
       </c>
@@ -70222,16 +70237,16 @@
         <v>37620000</v>
       </c>
       <c r="H19" s="80" cm="1">
-        <f t="array" ref="H19">SUM(_xlfn._xlws.FILTER('Usulan TUP 1'!$L$15:$L$564,'Usulan TUP 1'!$P$15:$P$564=D19,0))</f>
+        <f t="array" ref="H19">SUM(_xlfn._xlws.FILTER('Usulan TUP 1'!$L$15:$L$564,'Usulan TUP 1'!$P$15:$P$564=$D19,0))</f>
         <v>26565000</v>
       </c>
-      <c r="I19" s="191">
-        <f t="shared" si="3"/>
-        <v>26565000</v>
+      <c r="I19" s="191" cm="1">
+        <f t="array" ref="I19">SUM(_xlfn._xlws.FILTER('Usulan TUP 1'!$M$15:$M$564,'Usulan TUP 1'!$P$15:$P$564=$D19,0))</f>
+        <v>16416000</v>
       </c>
       <c r="J19" s="192">
         <f>H19-I19</f>
-        <v>0</v>
+        <v>10149000</v>
       </c>
       <c r="K19" s="31"/>
       <c r="L19" s="31"/>
@@ -70240,8 +70255,8 @@
       <c r="O19" s="31"/>
     </row>
     <row r="20" spans="2:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="308"/>
-      <c r="C20" s="309"/>
+      <c r="B20" s="306"/>
+      <c r="C20" s="331"/>
       <c r="D20" s="193" t="s">
         <v>531</v>
       </c>
@@ -70258,16 +70273,16 @@
         <v>126160000</v>
       </c>
       <c r="H20" s="195">
-        <f t="shared" ref="H20:J20" si="4">SUM(H18:H19)</f>
+        <f t="shared" ref="H20:J20" si="6">SUM(H18:H19)</f>
         <v>111105000</v>
       </c>
       <c r="I20" s="195">
-        <f t="shared" si="4"/>
-        <v>111105000</v>
+        <f t="shared" ref="I20" si="7">SUM(I18:I19)</f>
+        <v>75461795</v>
       </c>
       <c r="J20" s="195">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>35643205</v>
       </c>
       <c r="K20" s="81"/>
       <c r="L20" s="82"/>
@@ -70276,34 +70291,34 @@
       <c r="O20" s="31"/>
     </row>
     <row r="21" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="300" t="s">
+      <c r="B21" s="326" t="s">
         <v>532</v>
       </c>
-      <c r="C21" s="301"/>
-      <c r="D21" s="302"/>
+      <c r="C21" s="327"/>
+      <c r="D21" s="328"/>
       <c r="E21" s="198">
         <f>SUM(E11,E14,E17,E20)</f>
         <v>23288180000</v>
       </c>
       <c r="F21" s="198">
-        <f t="shared" ref="F21:J21" si="5">SUM(F11,F14,F17,F20)</f>
+        <f t="shared" ref="F21:J21" si="8">SUM(F11,F14,F17,F20)</f>
         <v>23083432654</v>
       </c>
       <c r="G21" s="198">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>334230000</v>
       </c>
       <c r="H21" s="197">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>267130000</v>
       </c>
       <c r="I21" s="197">
-        <f t="shared" si="5"/>
-        <v>120170000</v>
+        <f t="shared" ref="I21" si="9">SUM(I11,I14,I17,I20)</f>
+        <v>198046564</v>
       </c>
       <c r="J21" s="197">
-        <f t="shared" si="5"/>
-        <v>146960000</v>
+        <f t="shared" si="8"/>
+        <v>69083436</v>
       </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25"/>
@@ -71320,6 +71335,14 @@
     <row r="997" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="B9:B11"/>
     <mergeCell ref="B2:J2"/>
@@ -71334,18 +71357,10 @@
     <mergeCell ref="H6:H7"/>
     <mergeCell ref="I6:I7"/>
     <mergeCell ref="J6:J7"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C12:C14"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.59055118110236227" right="0.59055118110236227" top="0.74803149606299213" bottom="0.74803149606299213" header="0" footer="0.39370078740157483"/>
-  <pageSetup paperSize="9" scale="54" fitToHeight="0" pageOrder="overThenDown" orientation="portrait" cellComments="atEnd" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="55" fitToHeight="0" pageOrder="overThenDown" orientation="portrait" cellComments="atEnd" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Realisasi SP2D s.d 02 Maret 2023
</commit_message>
<xml_diff>
--- a/TUP/TUP 1/Usulan TUP 1.xlsx
+++ b/TUP/TUP 1/Usulan TUP 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BACK\PUSDIK\2023\Github\TA.2023\TUP\TUP 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{826DB08B-9BA1-474A-9C77-BEFBBB5C80F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9599379D-792A-4502-BFFC-0E0C73080332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E899FA34-6DE3-4640-B916-AC504F664995}"/>
   </bookViews>
@@ -154,7 +154,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId9"/>
+    <pivotCache cacheId="68" r:id="rId9"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -4958,6 +4958,26 @@
     <xf numFmtId="0" fontId="9" fillId="40" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="41" fontId="12" fillId="10" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="12" fillId="10" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="12" fillId="10" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -4965,8 +4985,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4983,11 +5001,9 @@
     <xf numFmtId="0" fontId="12" fillId="10" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5014,22 +5030,6 @@
     <xf numFmtId="0" fontId="15" fillId="9" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="41" fontId="12" fillId="10" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="12" fillId="10" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="12" fillId="10" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
@@ -5902,7 +5902,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$H$34:$H$35" spid="_x0000_s3412"/>
+                  <a14:cameraTool cellRange="$H$34:$H$35" spid="_x0000_s3419"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -8644,7 +8644,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1127F9CD-6ADB-4CE5-B7BF-433D4F60FD7D}" name="PivotTable10" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1127F9CD-6ADB-4CE5-B7BF-433D4F60FD7D}" name="PivotTable10" cacheId="68" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A11:D25" firstHeaderRow="0" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField name="Program, Kegiatan dan KRO" axis="axisRow" compact="0" outline="0" showAll="0">
@@ -10413,7 +10413,7 @@
   <dimension ref="A1:R965"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -37002,17 +37002,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16377" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="307" t="s">
+      <c r="B2" s="315" t="s">
         <v>985</v>
       </c>
-      <c r="C2" s="307"/>
-      <c r="D2" s="307"/>
-      <c r="E2" s="307"/>
-      <c r="F2" s="307"/>
-      <c r="G2" s="307"/>
-      <c r="H2" s="307"/>
-      <c r="I2" s="307"/>
-      <c r="J2" s="307"/>
+      <c r="C2" s="315"/>
+      <c r="D2" s="315"/>
+      <c r="E2" s="315"/>
+      <c r="F2" s="315"/>
+      <c r="G2" s="315"/>
+      <c r="H2" s="315"/>
+      <c r="I2" s="315"/>
+      <c r="J2" s="315"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
@@ -53382,17 +53382,17 @@
       <c r="XEW2" s="3"/>
     </row>
     <row r="3" spans="2:16377" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="308" t="s">
+      <c r="B3" s="316" t="s">
         <v>521</v>
       </c>
-      <c r="C3" s="308"/>
-      <c r="D3" s="308"/>
-      <c r="E3" s="308"/>
-      <c r="F3" s="308"/>
-      <c r="G3" s="308"/>
-      <c r="H3" s="308"/>
-      <c r="I3" s="308"/>
-      <c r="J3" s="308"/>
+      <c r="C3" s="316"/>
+      <c r="D3" s="316"/>
+      <c r="E3" s="316"/>
+      <c r="F3" s="316"/>
+      <c r="G3" s="316"/>
+      <c r="H3" s="316"/>
+      <c r="I3" s="316"/>
+      <c r="J3" s="316"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -69763,41 +69763,41 @@
     </row>
     <row r="4" spans="2:16377" x14ac:dyDescent="0.25"/>
     <row r="5" spans="2:16377" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="309" t="s">
+      <c r="B5" s="317" t="s">
         <v>522</v>
       </c>
-      <c r="C5" s="310"/>
+      <c r="C5" s="318"/>
       <c r="D5" s="20" t="s">
         <v>523</v>
       </c>
     </row>
     <row r="6" spans="2:16377" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="311" t="s">
+      <c r="B6" s="319" t="s">
         <v>524</v>
       </c>
-      <c r="C6" s="312" t="s">
+      <c r="C6" s="320" t="s">
         <v>525</v>
       </c>
-      <c r="D6" s="312" t="s">
+      <c r="D6" s="320" t="s">
         <v>526</v>
       </c>
-      <c r="E6" s="314" t="str">
+      <c r="E6" s="321" t="str">
         <f>"Pagu "</f>
         <v xml:space="preserve">Pagu </v>
       </c>
-      <c r="F6" s="316" t="s">
+      <c r="F6" s="322" t="s">
         <v>520</v>
       </c>
-      <c r="G6" s="318" t="s">
+      <c r="G6" s="324" t="s">
         <v>969</v>
       </c>
-      <c r="H6" s="320" t="s">
+      <c r="H6" s="326" t="s">
         <v>986</v>
       </c>
-      <c r="I6" s="322" t="s">
+      <c r="I6" s="328" t="s">
         <v>989</v>
       </c>
-      <c r="J6" s="324" t="s">
+      <c r="J6" s="330" t="s">
         <v>970</v>
       </c>
       <c r="K6" s="21"/>
@@ -69807,15 +69807,15 @@
       <c r="O6" s="21"/>
     </row>
     <row r="7" spans="2:16377" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="306"/>
-      <c r="C7" s="313"/>
-      <c r="D7" s="313"/>
-      <c r="E7" s="315"/>
-      <c r="F7" s="317"/>
-      <c r="G7" s="319"/>
-      <c r="H7" s="321"/>
-      <c r="I7" s="323"/>
-      <c r="J7" s="325"/>
+      <c r="B7" s="310"/>
+      <c r="C7" s="307"/>
+      <c r="D7" s="307"/>
+      <c r="E7" s="306"/>
+      <c r="F7" s="323"/>
+      <c r="G7" s="325"/>
+      <c r="H7" s="327"/>
+      <c r="I7" s="329"/>
+      <c r="J7" s="331"/>
       <c r="K7" s="21"/>
       <c r="L7" s="21"/>
       <c r="M7" s="21"/>
@@ -69826,10 +69826,10 @@
       <c r="B8" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="302" t="s">
+      <c r="C8" s="312" t="s">
         <v>527</v>
       </c>
-      <c r="D8" s="303"/>
+      <c r="D8" s="313"/>
       <c r="E8" s="23"/>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -69843,10 +69843,10 @@
       <c r="O8" s="25"/>
     </row>
     <row r="9" spans="2:16377" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="304">
+      <c r="B9" s="314">
         <v>1</v>
       </c>
-      <c r="C9" s="329" t="s">
+      <c r="C9" s="305" t="s">
         <v>500</v>
       </c>
       <c r="D9" s="26" t="s">
@@ -69883,8 +69883,8 @@
       <c r="O9" s="31"/>
     </row>
     <row r="10" spans="2:16377" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="305"/>
-      <c r="C10" s="315"/>
+      <c r="B10" s="309"/>
+      <c r="C10" s="306"/>
       <c r="D10" s="32" t="s">
         <v>502</v>
       </c>
@@ -69919,8 +69919,8 @@
       <c r="O10" s="31"/>
     </row>
     <row r="11" spans="2:16377" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="306"/>
-      <c r="C11" s="313"/>
+      <c r="B11" s="310"/>
+      <c r="C11" s="307"/>
       <c r="D11" s="60" t="s">
         <v>528</v>
       </c>
@@ -69955,10 +69955,10 @@
       <c r="O11" s="31"/>
     </row>
     <row r="12" spans="2:16377" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="330">
+      <c r="B12" s="308">
         <v>2</v>
       </c>
-      <c r="C12" s="329" t="s">
+      <c r="C12" s="305" t="s">
         <v>508</v>
       </c>
       <c r="D12" s="33" t="s">
@@ -69995,8 +69995,8 @@
       <c r="O12" s="31"/>
     </row>
     <row r="13" spans="2:16377" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="305"/>
-      <c r="C13" s="315"/>
+      <c r="B13" s="309"/>
+      <c r="C13" s="306"/>
       <c r="D13" s="33" t="s">
         <v>510</v>
       </c>
@@ -70031,8 +70031,8 @@
       <c r="O13" s="31"/>
     </row>
     <row r="14" spans="2:16377" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="306"/>
-      <c r="C14" s="313"/>
+      <c r="B14" s="310"/>
+      <c r="C14" s="307"/>
       <c r="D14" s="60" t="s">
         <v>529</v>
       </c>
@@ -70067,10 +70067,10 @@
       <c r="O14" s="31"/>
     </row>
     <row r="15" spans="2:16377" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="330">
+      <c r="B15" s="308">
         <v>3</v>
       </c>
-      <c r="C15" s="329" t="s">
+      <c r="C15" s="305" t="s">
         <v>503</v>
       </c>
       <c r="D15" s="33" t="s">
@@ -70107,8 +70107,8 @@
       <c r="O15" s="31"/>
     </row>
     <row r="16" spans="2:16377" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="305"/>
-      <c r="C16" s="315"/>
+      <c r="B16" s="309"/>
+      <c r="C16" s="306"/>
       <c r="D16" s="33" t="s">
         <v>505</v>
       </c>
@@ -70143,8 +70143,8 @@
       <c r="O16" s="31"/>
     </row>
     <row r="17" spans="2:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="306"/>
-      <c r="C17" s="313"/>
+      <c r="B17" s="310"/>
+      <c r="C17" s="307"/>
       <c r="D17" s="60" t="s">
         <v>530</v>
       </c>
@@ -70179,10 +70179,10 @@
       <c r="O17" s="31"/>
     </row>
     <row r="18" spans="2:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="330">
+      <c r="B18" s="308">
         <v>4</v>
       </c>
-      <c r="C18" s="329" t="s">
+      <c r="C18" s="305" t="s">
         <v>506</v>
       </c>
       <c r="D18" s="33" t="s">
@@ -70219,8 +70219,8 @@
       <c r="O18" s="31"/>
     </row>
     <row r="19" spans="2:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="305"/>
-      <c r="C19" s="315"/>
+      <c r="B19" s="309"/>
+      <c r="C19" s="306"/>
       <c r="D19" s="78" t="s">
         <v>511</v>
       </c>
@@ -70255,8 +70255,8 @@
       <c r="O19" s="31"/>
     </row>
     <row r="20" spans="2:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="306"/>
-      <c r="C20" s="331"/>
+      <c r="B20" s="310"/>
+      <c r="C20" s="311"/>
       <c r="D20" s="193" t="s">
         <v>531</v>
       </c>
@@ -70291,11 +70291,11 @@
       <c r="O20" s="31"/>
     </row>
     <row r="21" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="326" t="s">
+      <c r="B21" s="302" t="s">
         <v>532</v>
       </c>
-      <c r="C21" s="327"/>
-      <c r="D21" s="328"/>
+      <c r="C21" s="303"/>
+      <c r="D21" s="304"/>
       <c r="E21" s="198">
         <f>SUM(E11,E14,E17,E20)</f>
         <v>23288180000</v>
@@ -71335,14 +71335,6 @@
     <row r="997" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C12:C14"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="B9:B11"/>
     <mergeCell ref="B2:J2"/>
@@ -71357,6 +71349,14 @@
     <mergeCell ref="H6:H7"/>
     <mergeCell ref="I6:I7"/>
     <mergeCell ref="J6:J7"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.59055118110236227" right="0.59055118110236227" top="0.74803149606299213" bottom="0.74803149606299213" header="0" footer="0.39370078740157483"/>

</xml_diff>